<commit_message>
Found and fixed bug with construction of reaction to uniprot id dict in vis pathways. Brenda uniprot entries were actually multiple reactions wrapped in a list. Re-ran vis pathways on mvacid and hopa pathways to get more uniprot ids in excel sheets
</commit_message>
<xml_diff>
--- a/artifacts/pwy_xls/ccm_v0_to_hopa_gen_3_tan_sample_1_n_samples_1000.xlsx
+++ b/artifacts/pwy_xls/ccm_v0_to_hopa_gen_3_tan_sample_1_n_samples_1000.xlsx
@@ -494,13 +494,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A0PN13,A0PST9,A0QMB9,A0R4Q0,A1KF54,A1KJE8,A5TYV9,A5U390,B1XMM6,O32507,O69497,O85997,P25526,P38067,P55653,P94428,P9WNX6,P9WNX7,P9WNX8,Q0K2K1,Q4KKA2,Q55585,Q73TP5,Q7TZP3,Q9JTN7,Q9RBF6</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t xml:space="preserve">SUCCSEMIALDDEHYDROG-RXN_reverse: [A0PN13, A0PST9, A0QMB9, A0R4Q0, A1KF54, A1KJE8, A5TYV9, A5U390, B1XMM6, O32507, O69497, O85997, P25526, P38067, P55653, P94428, P9WNX6, P9WNX7, P9WNX8, Q0K2K1, Q4KKA2, Q55585, Q73TP5, Q7TZP3, Q9JTN7, Q9RBF6] | R00714_reverse: [] | 1.2.1.79 ()_6: [] | 1.2.1.24_53: [] | 1.2.1.16_25: [] | </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-11727: [] | R09545_reverse: [] | 1.1.1.308_0: [] | </t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>D0S1M8,P71362,Q1V6P8,Q43908;P26263;P26263,Q06408,Q07471;A2XFI3,A2Y5L9,A2YQ76,O42873,O82647,P16467,P26263,P28516,P33149,P33287,P34734,P51844,P51845,P51846,P51850,P51851,P83779,P87208,Q05326,Q05327,Q07471,Q09737,Q0CNV1,Q0D3D2,Q0DHF6,Q10MW3,Q12629,Q2UKV4,Q4WXX9,Q684J7,Q6FJA3,Q92345,Q9FFT4,Q9M039,Q9M040,Q9P7P6;P16467,P26263</t>
+          <t xml:space="preserve">R07650_reverse: [] | 4.1.1.86_0: [] | 4.1.1.86-RXN: [D0S1M8, P71362, Q1V6P8, Q43908] | R06614_reverse: [] | R00656_reverse: [] | METHIONINE-DECARBOXYLASE-RXN: [] | 4.1.1.57_2: [] | 4.1.1.14_03: [] | RXN-7704: [] | 4.1.1.72_19: [] | 4.1.1.43_05: [] | 4.1.1.1_19: [] | 4.1.1.86_4: [] | 4.1.1.72_33: [] | 4.1.1.43_11: [] | 4.1.1.1_38: [] | 4.1.1.72_34: [] | 4.1.1.1_39: [] | RXN-14985: [P26263] | 4.1.1.72_29: [] | 4.1.1.1_34: [] | 4.1.1.7_151: [] | 4.1.1.72_37: [] | 4.1.1.1_41: [] | R03894_reverse: [] | 4.1.1.7_062: [] | 4.1.1.72_04: [] | 4.1.1.72_03: [] | 4.1.1.72-RXN: [P26263, Q06408, Q07471] | 4.1.1.1_04: [] | VALINE-DECARBOXYLASE-RXN: [] | R01437_reverse: [] | 4.1.1.57_1: [] | 4.1.1.14_01: [] | RXN-7692: [A2XFI3, A2Y5L9, A2YQ76, O42873, O82647, P16467, P26263, P28516, P33149, P33287, P34734, P51844, P51845, P51846, P51850, P51851, P83779, P87208, Q05326, Q05327, Q07471, Q09737, Q0CNV1, Q0D3D2, Q0DHF6, Q10MW3, Q12629, Q2UKV4, Q4WXX9, Q684J7, Q6FJA3, Q92345, Q9FFT4, Q9M039, Q9M040, Q9P7P6] | 4.1.1.7_096: [] | 4.1.1.72_17: [] | 4.1.1.1_17: [] | RXN-7643: [P16467, P26263] | 4.1.1.7_145: [] | 4.1.1.72_32: [] | 4.1.1.1_37: [] | 2.2.1.6_12: [] | </t>
         </is>
       </c>
     </row>
@@ -524,15 +528,19 @@
       <c r="E3" t="n">
         <v>0.6154624613698966</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-11727: [] | R09545_reverse: [] | 1.1.1.308_0: [] | </t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>H8ZPX2</t>
+          <t xml:space="preserve">RXN-13089_reverse: [H8ZPX2] | </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>D0S1M8,P71362,Q1V6P8,Q43908;P26263;P26263,Q06408,Q07471;A2XFI3,A2Y5L9,A2YQ76,O42873,O82647,P16467,P26263,P28516,P33149,P33287,P34734,P51844,P51845,P51846,P51850,P51851,P83779,P87208,Q05326,Q05327,Q07471,Q09737,Q0CNV1,Q0D3D2,Q0DHF6,Q10MW3,Q12629,Q2UKV4,Q4WXX9,Q684J7,Q6FJA3,Q92345,Q9FFT4,Q9M039,Q9M040,Q9P7P6;P16467,P26263</t>
+          <t xml:space="preserve">R07650_reverse: [] | 4.1.1.86_0: [] | 4.1.1.86-RXN: [D0S1M8, P71362, Q1V6P8, Q43908] | R06614_reverse: [] | R00656_reverse: [] | METHIONINE-DECARBOXYLASE-RXN: [] | 4.1.1.57_2: [] | 4.1.1.14_03: [] | RXN-7704: [] | 4.1.1.72_19: [] | 4.1.1.43_05: [] | 4.1.1.1_19: [] | 4.1.1.86_4: [] | 4.1.1.72_33: [] | 4.1.1.43_11: [] | 4.1.1.1_38: [] | 4.1.1.72_34: [] | 4.1.1.1_39: [] | RXN-14985: [P26263] | 4.1.1.72_29: [] | 4.1.1.1_34: [] | 4.1.1.7_151: [] | 4.1.1.72_37: [] | 4.1.1.1_41: [] | R03894_reverse: [] | 4.1.1.7_062: [] | 4.1.1.72_04: [] | 4.1.1.72_03: [] | 4.1.1.72-RXN: [P26263, Q06408, Q07471] | 4.1.1.1_04: [] | VALINE-DECARBOXYLASE-RXN: [] | R01437_reverse: [] | 4.1.1.57_1: [] | 4.1.1.14_01: [] | RXN-7692: [A2XFI3, A2Y5L9, A2YQ76, O42873, O82647, P16467, P26263, P28516, P33149, P33287, P34734, P51844, P51845, P51846, P51850, P51851, P83779, P87208, Q05326, Q05327, Q07471, Q09737, Q0CNV1, Q0D3D2, Q0DHF6, Q10MW3, Q12629, Q2UKV4, Q4WXX9, Q684J7, Q6FJA3, Q92345, Q9FFT4, Q9M039, Q9M040, Q9P7P6] | 4.1.1.7_096: [] | 4.1.1.72_17: [] | 4.1.1.1_17: [] | RXN-7643: [P16467, P26263] | 4.1.1.7_145: [] | 4.1.1.72_32: [] | 4.1.1.1_37: [] | 2.2.1.6_12: [] | </t>
         </is>
       </c>
     </row>
@@ -612,13 +620,21 @@
       <c r="E2" t="n">
         <v>0.4912291941371058</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-11727: [] | R09545_reverse: [] | 1.1.1.308_0: [] | </t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>P02904,Q70AC7,Q8GBW6</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t xml:space="preserve">R00930_reverse: [] | 2.1.3.1_7: [] | 2.1.3.1-RXN: [P02904, Q70AC7, Q8GBW6] | </t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">R07219_reverse: [] | 1.17.7.4_1: [] | </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -642,11 +658,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>D5FKJ3</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t xml:space="preserve">RXN-14468_reverse: [] | 2.1.1.281 ()_1: [] | RXN-11456_reverse: [D5FKJ3] | R09939: [] | </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-16543_reverse: [] | </t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-14984: [] | RXN-14984_reverse: [] | </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -668,13 +692,21 @@
       <c r="E4" t="n">
         <v>0.4425101386765349</v>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-11727: [] | R09545_reverse: [] | 1.1.1.308_0: [] | </t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>D5FKJ3</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t xml:space="preserve">RXN-14468_reverse: [] | 2.1.1.281 ()_1: [] | RXN-11456_reverse: [D5FKJ3] | R09939: [] | </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-14984: [] | RXN-14984_reverse: [] | </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -754,15 +786,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Q88JX9</t>
+          <t xml:space="preserve">RXN-12074: [Q88JX9] | R00008_reverse: [] | 4.1.3.17_7: [] | 4.1.3.17-RXN: [] | </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A0AJ02,A0AJD9,A0B885,A0JYM2,A0K5D7,A0KNY9,A0KZS6,A0L3S9,A0LIP3,A0LRE5,A0LXY3,A0PLS0,A0Q2A8,A0Q628,A0QLG2,A0QR33,A0R9G6,A0RJ78,A0RQ51,A0RXB3,A1A7K0,A1ASE9,A1AVQ1,A1BJG8,A1JJQ1,A1KB59,A1KG00,A1KS34,A1R898,A1RMG7,A1RQR5,A1S3U0,A1SE06,A1ST92,A1T3F2,A1TKK8,A1TYG5,A1UAR1,A1V1L0,A1V9X6,A1VSM6,A1VZJ6,A1WBR8,A1WMA0,A1WYL3,A2BL27,A2BPW6,A2BVE5,A2C0U2,A2C7I7,A2S9D9,A2SKQ7,A2SQU3,A3CL81,A3CU65,A3D1R5,A3DIF3,A3M7I8,A3MMQ8,A3MWW7,A3N2K3,A3NCF3,A3NY82,A3PBK8,A3PUB7,A3QBN5,A4FPX3,A4FZY1,A4G8N0,A4IKL1,A4IRG2,A4IXN8,A4J6H0,A4JC86,A4QB78,A4SGT2,A4SJ79,A4SVE6,A4T358,A4TPW6,A4VQY0,A4W6Q1,A4WN33,A4XC73,A4XK09,A4XYV6,A4Y4G4,A4YD91,A5CNI7,A5CXH8,A5D3M2,A5EXX1,A5F945,A5FIM3,A5G9C0,A5GMT2,A5GUJ2,A5IC29,A5ITJ2,A5IU30,A5N5Y1,A5TZQ4,A5UML0,A5UU40,A5VM65,A5W9H0,A5WC94,A6GYW4,A6LKX4,A6LSY8,A6Q2X6,A6Q9P9,A6QHK1,A6QI46,A6T2A2,A6T4V8,A6TJD8,A6U2D5,A6U2W8,A6URL2,A6UWB3,A6V0D2,A6VIL1,A6VQ66,A6VUX8,A6W5M6,A6WKL6,A7FM09,A7GL00,A7GTE2,A7GXK4,A7H3N1,A7HIX3,A7I252,A7I7P2,A7MGR5,A7MUU9,A7NCX8,A7NKV1,A7X388,A7X3X9,A7Z2N8,A7Z7A2,A7ZCH5,A7ZHP6,A7ZWA2,A8AAB3,A8ALD5,A8ETJ2,A8FB92,A8FFU9,A8FLR2,A8FS76,A8G3J9,A8G9U7,A8H164,A8LCD0,A8M6S5,A8M919,A8MGY8,A8YY36,A8Z2I8,A8ZZU9,A9A1A0,A9A875,A9AEU0,A9B550,A9BEA5,A9BY74,A9GDD3,A9I1R3,A9KBA0,A9KP86,A9KSC7,A9L5J5,A9M1G6,A9MPK7,A9N0P9,A9NAX3,A9R1E6,A9VIT5,A9VSS7,A9WIS7,A9WPI0,B0B9W0,B0BBJ0,B0BRF0,B0CC57,B0JPW6,B0KJV9,B0R7L9,B0RBL3,B0RP74,B0SF64,B0SNK3,B0TFV0,B0TIQ0,B0U0T6,B0U328,B0UST3,B0VCN6,B0VU92,B1HUT1,B1HVD3,B1I4L1,B1IQI6,B1J1Y6,B1JK22,B1JX81,B1KHF6,B1LGV7,B1MHH1,B1VEK3,B1VTD1,B1X023,B1XD24,B1XIT5,B1XT79,B1Y8G2,B1YBL3,B1YJU8,B1YK58,B1YUJ7,B1ZVF7,B2A1H4,B2FT35,B2G9H2,B2GL27,B2HRL5,B2HW19,B2I6C2,B2J7M9,B2JED5,B2K547,B2SGG7,B2SKS0,B2T6C2,B2TPD4,B2U2Z9,B2U6Q7,B2UNE3,B2USD7,B2UX41,B2V5U0,B2VE25,B3DY05,B3E9X0,B3EI07,B3EKJ7,B3GYN8,B3PL68,B3QRD2,B3QSA6,B3R312,B4EBT3,B4EUE1,B4RNX2,B4S0D0,B4S3Q6,B4SGW1,B4SI23,B4SUY4,B4TK30,B4TXQ6,B4U8M6,B4UKE6,B5BL82,B5EFG4,B5ERN9,B5F8R5,B5FAL8,B5FJ01,B5R3G6,B5RHE0,B5Y1L5,B5YHH6,B5Z0D4,B5ZA72,B6EL04,B6HZD0,B6J3H2,B6J495,B6JKN5,B7GH35,B7GIK0,B7GYZ5,B7H9S6,B7HE93,B7HQM1,B7HU66,B7I4N4,B7IHH3,B7IIX2,B7IW22,B7JBI1,B7JNG6,B7JQ54,B7K2I1,B7KA18,B7LGL6,B7LWB5,B7M195,B7MBD7,B7MP16,B7N823,B7NIB7,B7UIK1,B7V9D9,B7VJJ5,B8CJG4,B8DFN7,B8DHJ5,B8DN02,B8EBU3,B8F7H5,B8FBA1,B8G2L6,B8G822,B8GJJ2,B8GLE4,B8HBR2,B8HYK1,B8I0R1,B8J3A3,B8JCU6,B8ZT67,B9DMX3,B9DND8,B9DZG0,B9E740,B9E7Y3,B9IZ36,B9J3N2,B9KFS8,B9L0Q2,B9LA83,B9LKS0,B9LTZ9,B9LZL6,B9MF68,B9MRJ7,C0Q5R5,C0QCR9,C0QQ98,C0Z671,C0ZAH4,C0ZUX9,C1A7K7,C1AKK4,C1AZ30,C1CWI8,C1D9B6,C1DMY5,C1DUY4,C1ETQ7,C1EWG6,C1F911,C1KVK0,C1KVY4,C3K2K3,C3L6Z2,C3LHA0,C3LSN1,C3MJ22,C3MYE0,C3MZR9,C3N842,C3NF69,C3P9E6,C3PCZ3,C3PKI4,C4K6Y5,C4KJ00,C4L367,C4L4J9,C4LAK4,C4ZRP7,C5BAP9,C6AR33,C6DC32,E1W874,O26330,O29027,O66998,O74038,O74061,O84212,P0C1P8,P0C2D9,P0CL07,P18492,P21267,P23893,P24630,P30949,P31593,P45621,P46716,P48247,P56115,P63507,P63508,P71084,P99096,P9WMN8,P9WMN9,Q01YQ2,Q02SE5,Q04NV4,Q04X52,Q06741,Q06774,Q07YU5,Q0AAH7,Q0AFV1,Q0AZ36,Q0BHJ2,Q0BLC7,Q0HG53,Q0HSE6,Q0I3R7,Q0I8G1,Q0KDN9,Q0RS03,Q0SF42,Q0ST19,Q0T852,Q0TLH7,Q0TQG7,Q0VSP6,Q0W5T3,Q110Z9,Q11WK1,Q12EF7,Q12KC8,Q12WM7,Q13V40,Q14HS1,Q15YL3,Q17X40,Q18ES5,Q1AUK6,Q1BE73,Q1BYB1,Q1C3X1,Q1CLU7,Q1CUJ7,Q1DFA7,Q1GXW0,Q1I4H5,Q1IHV2,Q1IWZ8,Q1LQM3,Q1MPW7,Q1QEE8,Q1QSB0,Q1RG34,Q21MJ0,Q21YQ0,Q24VD4,Q254Z2,Q2A2U8,Q2FFN1,Q2FG69,Q2FTK5,Q2FXR4,Q2G283,Q2IHP8,Q2JFQ1,Q2JMP7,Q2JS70,Q2KUS4,Q2LVW6,Q2NF42,Q2NVQ0,Q2P6E4,Q2RJ31,Q2S1S3,Q2S8X9,Q2SYB2,Q2Y5Q5,Q2YTC2,Q2YU22,Q30RJ4,Q30WH2,Q31C50,Q31FB1,Q31QJ2,Q325Y5,Q32JV4,Q39566,Q39IQ4,Q39QA6,Q3A7W5,Q3ACS9,Q3ALU9,Q3AP59,Q3AWP4,Q3B1A1,Q3BPP7,Q3IHS1,Q3IT20,Q3JDH7,Q3JPN1,Q3K6C0,Q3KMF2,Q3M3B9,Q3SFU6,Q3Z5K3,Q40147,Q42522,Q46CH1,Q46GT9,Q46XZ7,Q478V1,Q47LB3,Q47V96,Q48DP1,Q49Y99,Q49YQ9,Q4FVC4,Q4JAM7,Q4JSY1,Q4K5I6,Q4L706,Q4L7G9,Q4UYA7,Q4ZNA0,Q55665,Q57T53,Q58020,Q5E2W6,Q5FAH9,Q5H3I5,Q5HER0,Q5HFA5,Q5HN71,Q5HNN6,Q5HUU3,Q5KWK9,Q5L2S4,Q5L5P0,Q5NGB9,Q5P6J6,Q5PD43,Q5QVP9,Q5SJS4,Q5UZ90,Q5WEP8,Q5WIE9,Q5WWG1,Q5X529,Q5YP79,Q5ZVA6,Q60CV0,Q62HV8,Q633Y3,Q63GB4,Q63RP8,Q65GK4,Q65M82,Q65U43,Q66EF1,Q67KM3,Q6AB08,Q6AHE8,Q6AQ32,Q6D1Z0,Q6FCY1,Q6G870,Q6G8Q8,Q6GFJ3,Q6GG38,Q6HD65,Q6HNS8,Q6L2G9,Q6LUS3,Q6M0P5,Q6MAC7,Q6MHT9,Q6NJJ2,Q6YZE2,Q71YY2,Q71ZB5,Q725I1,Q72K83,Q72ZW5,Q73DX4,Q73SQ3,Q74GA9,Q75G04,Q7A4T5,Q7M847,Q7MHY9,Q7N845,Q7NPI4,Q7P1Z5,Q7U598,Q7UPM9,Q7V2J3,Q7V677,Q7VDA1,Q7VHK3,Q7W050,Q7W3U1,Q7WF71,Q817R3,Q81I85,Q81LD0,Q81YV0,Q821C1,Q822Q0,Q82E21,Q82UQ8,Q83AK3,Q83FJ5,Q83H98,Q85WB7,Q87BW3,Q87LY3,Q87VY5,Q88DP0,Q897K4,Q8CNZ1,Q8CRW7,Q8CV56,Q8CZE3,Q8D3C8,Q8DBX8,Q8DLK8,Q8EHC8,Q8EY44,Q8FL16,Q8FSD4,Q8KAQ7,Q8NT73,Q8NVU6,Q8NW75,Q8P5R4,Q8PH40,Q8PW58,Q8RFY7,Q8TT57,Q8TYL6,Q8X4V5,Q8Y1M4,Q8Y6J9,Q8Y6X8,Q8YS26,Q8Z9B4,Q8ZBL9,Q8ZYW1,Q92AX5,Q92BG1,Q976H2,Q97B25,Q97MU2,Q980U5,Q99T15,Q9CNG9,Q9F2S0,Q9HKM6,Q9HMY8,Q9JRW9,Q9JW10,Q9JXW0,Q9K8G3,Q9KEB0,Q9KU97,Q9PB43,Q9PKI3,Q9PP70,Q9RWW0,Q9Y9I9,Q9ZMD0</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t xml:space="preserve">R02272: [] | GSAAMINOTRANS-RXN: [A0AJ02, A0AJD9, A0B885, A0JYM2, A0K5D7, A0KNY9, A0KZS6, A0L3S9, A0LIP3, A0LRE5, A0LXY3, A0PLS0, A0Q2A8, A0Q628, A0QLG2, A0QR33, A0R9G6, A0RJ78, A0RQ51, A0RXB3, A1A7K0, A1ASE9, A1AVQ1, A1BJG8, A1JJQ1, A1KB59, A1KG00, A1KS34, A1R898, A1RMG7, A1RQR5, A1S3U0, A1SE06, A1ST92, A1T3F2, A1TKK8, A1TYG5, A1UAR1, A1V1L0, A1V9X6, A1VSM6, A1VZJ6, A1WBR8, A1WMA0, A1WYL3, A2BL27, A2BPW6, A2BVE5, A2C0U2, A2C7I7, A2S9D9, A2SKQ7, A2SQU3, A3CL81, A3CU65, A3D1R5, A3DIF3, A3M7I8, A3MMQ8, A3MWW7, A3N2K3, A3NCF3, A3NY82, A3PBK8, A3PUB7, A3QBN5, A4FPX3, A4FZY1, A4G8N0, A4IKL1, A4IRG2, A4IXN8, A4J6H0, A4JC86, A4QB78, A4SGT2, A4SJ79, A4SVE6, A4T358, A4TPW6, A4VQY0, A4W6Q1, A4WN33, A4XC73, A4XK09, A4XYV6, A4Y4G4, A4YD91, A5CNI7, A5CXH8, A5D3M2, A5EXX1, A5F945, A5FIM3, A5G9C0, A5GMT2, A5GUJ2, A5IC29, A5ITJ2, A5IU30, A5N5Y1, A5TZQ4, A5UML0, A5UU40, A5VM65, A5W9H0, A5WC94, A6GYW4, A6LKX4, A6LSY8, A6Q2X6, A6Q9P9, A6QHK1, A6QI46, A6T2A2, A6T4V8, A6TJD8, A6U2D5, A6U2W8, A6URL2, A6UWB3, A6V0D2, A6VIL1, A6VQ66, A6VUX8, A6W5M6, A6WKL6, A7FM09, A7GL00, A7GTE2, A7GXK4, A7H3N1, A7HIX3, A7I252, A7I7P2, A7MGR5, A7MUU9, A7NCX8, A7NKV1, A7X388, A7X3X9, A7Z2N8, A7Z7A2, A7ZCH5, A7ZHP6, A7ZWA2, A8AAB3, A8ALD5, A8ETJ2, A8FB92, A8FFU9, A8FLR2, A8FS76, A8G3J9, A8G9U7, A8H164, A8LCD0, A8M6S5, A8M919, A8MGY8, A8YY36, A8Z2I8, A8ZZU9, A9A1A0, A9A875, A9AEU0, A9B550, A9BEA5, A9BY74, A9GDD3, A9I1R3, A9KBA0, A9KP86, A9KSC7, A9L5J5, A9M1G6, A9MPK7, A9N0P9, A9NAX3, A9R1E6, A9VIT5, A9VSS7, A9WIS7, A9WPI0, B0B9W0, B0BBJ0, B0BRF0, B0CC57, B0JPW6, B0KJV9, B0R7L9, B0RBL3, B0RP74, B0SF64, B0SNK3, B0TFV0, B0TIQ0, B0U0T6, B0U328, B0UST3, B0VCN6, B0VU92, B1HUT1, B1HVD3, B1I4L1, B1IQI6, B1J1Y6, B1JK22, B1JX81, B1KHF6, B1LGV7, B1MHH1, B1VEK3, B1VTD1, B1X023, B1XD24, B1XIT5, B1XT79, B1Y8G2, B1YBL3, B1YJU8, B1YK58, B1YUJ7, B1ZVF7, B2A1H4, B2FT35, B2G9H2, B2GL27, B2HRL5, B2HW19, B2I6C2, B2J7M9, B2JED5, B2K547, B2SGG7, B2SKS0, B2T6C2, B2TPD4, B2U2Z9, B2U6Q7, B2UNE3, B2USD7, B2UX41, B2V5U0, B2VE25, B3DY05, B3E9X0, B3EI07, B3EKJ7, B3GYN8, B3PL68, B3QRD2, B3QSA6, B3R312, B4EBT3, B4EUE1, B4RNX2, B4S0D0, B4S3Q6, B4SGW1, B4SI23, B4SUY4, B4TK30, B4TXQ6, B4U8M6, B4UKE6, B5BL82, B5EFG4, B5ERN9, B5F8R5, B5FAL8, B5FJ01, B5R3G6, B5RHE0, B5Y1L5, B5YHH6, B5Z0D4, B5ZA72, B6EL04, B6HZD0, B6J3H2, B6J495, B6JKN5, B7GH35, B7GIK0, B7GYZ5, B7H9S6, B7HE93, B7HQM1, B7HU66, B7I4N4, B7IHH3, B7IIX2, B7IW22, B7JBI1, B7JNG6, B7JQ54, B7K2I1, B7KA18, B7LGL6, B7LWB5, B7M195, B7MBD7, B7MP16, B7N823, B7NIB7, B7UIK1, B7V9D9, B7VJJ5, B8CJG4, B8DFN7, B8DHJ5, B8DN02, B8EBU3, B8F7H5, B8FBA1, B8G2L6, B8G822, B8GJJ2, B8GLE4, B8HBR2, B8HYK1, B8I0R1, B8J3A3, B8JCU6, B8ZT67, B9DMX3, B9DND8, B9DZG0, B9E740, B9E7Y3, B9IZ36, B9J3N2, B9KFS8, B9L0Q2, B9LA83, B9LKS0, B9LTZ9, B9LZL6, B9MF68, B9MRJ7, C0Q5R5, C0QCR9, C0QQ98, C0Z671, C0ZAH4, C0ZUX9, C1A7K7, C1AKK4, C1AZ30, C1CWI8, C1D9B6, C1DMY5, C1DUY4, C1ETQ7, C1EWG6, C1F911, C1KVK0, C1KVY4, C3K2K3, C3L6Z2, C3LHA0, C3LSN1, C3MJ22, C3MYE0, C3MZR9, C3N842, C3NF69, C3P9E6, C3PCZ3, C3PKI4, C4K6Y5, C4KJ00, C4L367, C4L4J9, C4LAK4, C4ZRP7, C5BAP9, C6AR33, C6DC32, E1W874, O26330, O29027, O66998, O74038, O74061, O84212, P0C1P8, P0C2D9, P0CL07, P18492, P21267, P23893, P24630, P30949, P31593, P45621, P46716, P48247, P56115, P63507, P63508, P71084, P99096, P9WMN8, P9WMN9, Q01YQ2, Q02SE5, Q04NV4, Q04X52, Q06741, Q06774, Q07YU5, Q0AAH7, Q0AFV1, Q0AZ36, Q0BHJ2, Q0BLC7, Q0HG53, Q0HSE6, Q0I3R7, Q0I8G1, Q0KDN9, Q0RS03, Q0SF42, Q0ST19, Q0T852, Q0TLH7, Q0TQG7, Q0VSP6, Q0W5T3, Q110Z9, Q11WK1, Q12EF7, Q12KC8, Q12WM7, Q13V40, Q14HS1, Q15YL3, Q17X40, Q18ES5, Q1AUK6, Q1BE73, Q1BYB1, Q1C3X1, Q1CLU7, Q1CUJ7, Q1DFA7, Q1GXW0, Q1I4H5, Q1IHV2, Q1IWZ8, Q1LQM3, Q1MPW7, Q1QEE8, Q1QSB0, Q1RG34, Q21MJ0, Q21YQ0, Q24VD4, Q254Z2, Q2A2U8, Q2FFN1, Q2FG69, Q2FTK5, Q2FXR4, Q2G283, Q2IHP8, Q2JFQ1, Q2JMP7, Q2JS70, Q2KUS4, Q2LVW6, Q2NF42, Q2NVQ0, Q2P6E4, Q2RJ31, Q2S1S3, Q2S8X9, Q2SYB2, Q2Y5Q5, Q2YTC2, Q2YU22, Q30RJ4, Q30WH2, Q31C50, Q31FB1, Q31QJ2, Q325Y5, Q32JV4, Q39566, Q39IQ4, Q39QA6, Q3A7W5, Q3ACS9, Q3ALU9, Q3AP59, Q3AWP4, Q3B1A1, Q3BPP7, Q3IHS1, Q3IT20, Q3JDH7, Q3JPN1, Q3K6C0, Q3KMF2, Q3M3B9, Q3SFU6, Q3Z5K3, Q40147, Q42522, Q46CH1, Q46GT9, Q46XZ7, Q478V1, Q47LB3, Q47V96, Q48DP1, Q49Y99, Q49YQ9, Q4FVC4, Q4JAM7, Q4JSY1, Q4K5I6, Q4L706, Q4L7G9, Q4UYA7, Q4ZNA0, Q55665, Q57T53, Q58020, Q5E2W6, Q5FAH9, Q5H3I5, Q5HER0, Q5HFA5, Q5HN71, Q5HNN6, Q5HUU3, Q5KWK9, Q5L2S4, Q5L5P0, Q5NGB9, Q5P6J6, Q5PD43, Q5QVP9, Q5SJS4, Q5UZ90, Q5WEP8, Q5WIE9, Q5WWG1, Q5X529, Q5YP79, Q5ZVA6, Q60CV0, Q62HV8, Q633Y3, Q63GB4, Q63RP8, Q65GK4, Q65M82, Q65U43, Q66EF1, Q67KM3, Q6AB08, Q6AHE8, Q6AQ32, Q6D1Z0, Q6FCY1, Q6G870, Q6G8Q8, Q6GFJ3, Q6GG38, Q6HD65, Q6HNS8, Q6L2G9, Q6LUS3, Q6M0P5, Q6MAC7, Q6MHT9, Q6NJJ2, Q6YZE2, Q71YY2, Q71ZB5, Q725I1, Q72K83, Q72ZW5, Q73DX4, Q73SQ3, Q74GA9, Q75G04, Q7A4T5, Q7M847, Q7MHY9, Q7N845, Q7NPI4, Q7P1Z5, Q7U598, Q7UPM9, Q7V2J3, Q7V677, Q7VDA1, Q7VHK3, Q7W050, Q7W3U1, Q7WF71, Q817R3, Q81I85, Q81LD0, Q81YV0, Q821C1, Q822Q0, Q82E21, Q82UQ8, Q83AK3, Q83FJ5, Q83H98, Q85WB7, Q87BW3, Q87LY3, Q87VY5, Q88DP0, Q897K4, Q8CNZ1, Q8CRW7, Q8CV56, Q8CZE3, Q8D3C8, Q8DBX8, Q8DLK8, Q8EHC8, Q8EY44, Q8FL16, Q8FSD4, Q8KAQ7, Q8NT73, Q8NVU6, Q8NW75, Q8P5R4, Q8PH40, Q8PW58, Q8RFY7, Q8TT57, Q8TYL6, Q8X4V5, Q8Y1M4, Q8Y6J9, Q8Y6X8, Q8YS26, Q8Z9B4, Q8ZBL9, Q8ZYW1, Q92AX5, Q92BG1, Q976H2, Q97B25, Q97MU2, Q980U5, Q99T15, Q9CNG9, Q9F2S0, Q9HKM6, Q9HMY8, Q9JRW9, Q9JW10, Q9JXW0, Q9K8G3, Q9KEB0, Q9KU97, Q9PB43, Q9PKI3, Q9PP70, Q9RWW0, Q9Y9I9, Q9ZMD0] | 5.4.3.8_1: [] | </t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RXN-17561_reverse: [] | </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -786,17 +822,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Q88JX9</t>
+          <t xml:space="preserve">RXN-12074: [Q88JX9] | R00008_reverse: [] | 4.1.3.17_7: [] | 4.1.3.17-RXN: [] | </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A0AJ02,A0AJD9,A0B885,A0JYM2,A0K5D7,A0KNY9,A0KZS6,A0L3S9,A0LIP3,A0LRE5,A0LXY3,A0PLS0,A0Q2A8,A0Q628,A0QLG2,A0QR33,A0R9G6,A0RJ78,A0RQ51,A0RXB3,A1A7K0,A1ASE9,A1AVQ1,A1BJG8,A1JJQ1,A1KB59,A1KG00,A1KS34,A1R898,A1RMG7,A1RQR5,A1S3U0,A1SE06,A1ST92,A1T3F2,A1TKK8,A1TYG5,A1UAR1,A1V1L0,A1V9X6,A1VSM6,A1VZJ6,A1WBR8,A1WMA0,A1WYL3,A2BL27,A2BPW6,A2BVE5,A2C0U2,A2C7I7,A2S9D9,A2SKQ7,A2SQU3,A3CL81,A3CU65,A3D1R5,A3DIF3,A3M7I8,A3MMQ8,A3MWW7,A3N2K3,A3NCF3,A3NY82,A3PBK8,A3PUB7,A3QBN5,A4FPX3,A4FZY1,A4G8N0,A4IKL1,A4IRG2,A4IXN8,A4J6H0,A4JC86,A4QB78,A4SGT2,A4SJ79,A4SVE6,A4T358,A4TPW6,A4VQY0,A4W6Q1,A4WN33,A4XC73,A4XK09,A4XYV6,A4Y4G4,A4YD91,A5CNI7,A5CXH8,A5D3M2,A5EXX1,A5F945,A5FIM3,A5G9C0,A5GMT2,A5GUJ2,A5IC29,A5ITJ2,A5IU30,A5N5Y1,A5TZQ4,A5UML0,A5UU40,A5VM65,A5W9H0,A5WC94,A6GYW4,A6LKX4,A6LSY8,A6Q2X6,A6Q9P9,A6QHK1,A6QI46,A6T2A2,A6T4V8,A6TJD8,A6U2D5,A6U2W8,A6URL2,A6UWB3,A6V0D2,A6VIL1,A6VQ66,A6VUX8,A6W5M6,A6WKL6,A7FM09,A7GL00,A7GTE2,A7GXK4,A7H3N1,A7HIX3,A7I252,A7I7P2,A7MGR5,A7MUU9,A7NCX8,A7NKV1,A7X388,A7X3X9,A7Z2N8,A7Z7A2,A7ZCH5,A7ZHP6,A7ZWA2,A8AAB3,A8ALD5,A8ETJ2,A8FB92,A8FFU9,A8FLR2,A8FS76,A8G3J9,A8G9U7,A8H164,A8LCD0,A8M6S5,A8M919,A8MGY8,A8YY36,A8Z2I8,A8ZZU9,A9A1A0,A9A875,A9AEU0,A9B550,A9BEA5,A9BY74,A9GDD3,A9I1R3,A9KBA0,A9KP86,A9KSC7,A9L5J5,A9M1G6,A9MPK7,A9N0P9,A9NAX3,A9R1E6,A9VIT5,A9VSS7,A9WIS7,A9WPI0,B0B9W0,B0BBJ0,B0BRF0,B0CC57,B0JPW6,B0KJV9,B0R7L9,B0RBL3,B0RP74,B0SF64,B0SNK3,B0TFV0,B0TIQ0,B0U0T6,B0U328,B0UST3,B0VCN6,B0VU92,B1HUT1,B1HVD3,B1I4L1,B1IQI6,B1J1Y6,B1JK22,B1JX81,B1KHF6,B1LGV7,B1MHH1,B1VEK3,B1VTD1,B1X023,B1XD24,B1XIT5,B1XT79,B1Y8G2,B1YBL3,B1YJU8,B1YK58,B1YUJ7,B1ZVF7,B2A1H4,B2FT35,B2G9H2,B2GL27,B2HRL5,B2HW19,B2I6C2,B2J7M9,B2JED5,B2K547,B2SGG7,B2SKS0,B2T6C2,B2TPD4,B2U2Z9,B2U6Q7,B2UNE3,B2USD7,B2UX41,B2V5U0,B2VE25,B3DY05,B3E9X0,B3EI07,B3EKJ7,B3GYN8,B3PL68,B3QRD2,B3QSA6,B3R312,B4EBT3,B4EUE1,B4RNX2,B4S0D0,B4S3Q6,B4SGW1,B4SI23,B4SUY4,B4TK30,B4TXQ6,B4U8M6,B4UKE6,B5BL82,B5EFG4,B5ERN9,B5F8R5,B5FAL8,B5FJ01,B5R3G6,B5RHE0,B5Y1L5,B5YHH6,B5Z0D4,B5ZA72,B6EL04,B6HZD0,B6J3H2,B6J495,B6JKN5,B7GH35,B7GIK0,B7GYZ5,B7H9S6,B7HE93,B7HQM1,B7HU66,B7I4N4,B7IHH3,B7IIX2,B7IW22,B7JBI1,B7JNG6,B7JQ54,B7K2I1,B7KA18,B7LGL6,B7LWB5,B7M195,B7MBD7,B7MP16,B7N823,B7NIB7,B7UIK1,B7V9D9,B7VJJ5,B8CJG4,B8DFN7,B8DHJ5,B8DN02,B8EBU3,B8F7H5,B8FBA1,B8G2L6,B8G822,B8GJJ2,B8GLE4,B8HBR2,B8HYK1,B8I0R1,B8J3A3,B8JCU6,B8ZT67,B9DMX3,B9DND8,B9DZG0,B9E740,B9E7Y3,B9IZ36,B9J3N2,B9KFS8,B9L0Q2,B9LA83,B9LKS0,B9LTZ9,B9LZL6,B9MF68,B9MRJ7,C0Q5R5,C0QCR9,C0QQ98,C0Z671,C0ZAH4,C0ZUX9,C1A7K7,C1AKK4,C1AZ30,C1CWI8,C1D9B6,C1DMY5,C1DUY4,C1ETQ7,C1EWG6,C1F911,C1KVK0,C1KVY4,C3K2K3,C3L6Z2,C3LHA0,C3LSN1,C3MJ22,C3MYE0,C3MZR9,C3N842,C3NF69,C3P9E6,C3PCZ3,C3PKI4,C4K6Y5,C4KJ00,C4L367,C4L4J9,C4LAK4,C4ZRP7,C5BAP9,C6AR33,C6DC32,E1W874,O26330,O29027,O66998,O74038,O74061,O84212,P0C1P8,P0C2D9,P0CL07,P18492,P21267,P23893,P24630,P30949,P31593,P45621,P46716,P48247,P56115,P63507,P63508,P71084,P99096,P9WMN8,P9WMN9,Q01YQ2,Q02SE5,Q04NV4,Q04X52,Q06741,Q06774,Q07YU5,Q0AAH7,Q0AFV1,Q0AZ36,Q0BHJ2,Q0BLC7,Q0HG53,Q0HSE6,Q0I3R7,Q0I8G1,Q0KDN9,Q0RS03,Q0SF42,Q0ST19,Q0T852,Q0TLH7,Q0TQG7,Q0VSP6,Q0W5T3,Q110Z9,Q11WK1,Q12EF7,Q12KC8,Q12WM7,Q13V40,Q14HS1,Q15YL3,Q17X40,Q18ES5,Q1AUK6,Q1BE73,Q1BYB1,Q1C3X1,Q1CLU7,Q1CUJ7,Q1DFA7,Q1GXW0,Q1I4H5,Q1IHV2,Q1IWZ8,Q1LQM3,Q1MPW7,Q1QEE8,Q1QSB0,Q1RG34,Q21MJ0,Q21YQ0,Q24VD4,Q254Z2,Q2A2U8,Q2FFN1,Q2FG69,Q2FTK5,Q2FXR4,Q2G283,Q2IHP8,Q2JFQ1,Q2JMP7,Q2JS70,Q2KUS4,Q2LVW6,Q2NF42,Q2NVQ0,Q2P6E4,Q2RJ31,Q2S1S3,Q2S8X9,Q2SYB2,Q2Y5Q5,Q2YTC2,Q2YU22,Q30RJ4,Q30WH2,Q31C50,Q31FB1,Q31QJ2,Q325Y5,Q32JV4,Q39566,Q39IQ4,Q39QA6,Q3A7W5,Q3ACS9,Q3ALU9,Q3AP59,Q3AWP4,Q3B1A1,Q3BPP7,Q3IHS1,Q3IT20,Q3JDH7,Q3JPN1,Q3K6C0,Q3KMF2,Q3M3B9,Q3SFU6,Q3Z5K3,Q40147,Q42522,Q46CH1,Q46GT9,Q46XZ7,Q478V1,Q47LB3,Q47V96,Q48DP1,Q49Y99,Q49YQ9,Q4FVC4,Q4JAM7,Q4JSY1,Q4K5I6,Q4L706,Q4L7G9,Q4UYA7,Q4ZNA0,Q55665,Q57T53,Q58020,Q5E2W6,Q5FAH9,Q5H3I5,Q5HER0,Q5HFA5,Q5HN71,Q5HNN6,Q5HUU3,Q5KWK9,Q5L2S4,Q5L5P0,Q5NGB9,Q5P6J6,Q5PD43,Q5QVP9,Q5SJS4,Q5UZ90,Q5WEP8,Q5WIE9,Q5WWG1,Q5X529,Q5YP79,Q5ZVA6,Q60CV0,Q62HV8,Q633Y3,Q63GB4,Q63RP8,Q65GK4,Q65M82,Q65U43,Q66EF1,Q67KM3,Q6AB08,Q6AHE8,Q6AQ32,Q6D1Z0,Q6FCY1,Q6G870,Q6G8Q8,Q6GFJ3,Q6GG38,Q6HD65,Q6HNS8,Q6L2G9,Q6LUS3,Q6M0P5,Q6MAC7,Q6MHT9,Q6NJJ2,Q6YZE2,Q71YY2,Q71ZB5,Q725I1,Q72K83,Q72ZW5,Q73DX4,Q73SQ3,Q74GA9,Q75G04,Q7A4T5,Q7M847,Q7MHY9,Q7N845,Q7NPI4,Q7P1Z5,Q7U598,Q7UPM9,Q7V2J3,Q7V677,Q7VDA1,Q7VHK3,Q7W050,Q7W3U1,Q7WF71,Q817R3,Q81I85,Q81LD0,Q81YV0,Q821C1,Q822Q0,Q82E21,Q82UQ8,Q83AK3,Q83FJ5,Q83H98,Q85WB7,Q87BW3,Q87LY3,Q87VY5,Q88DP0,Q897K4,Q8CNZ1,Q8CRW7,Q8CV56,Q8CZE3,Q8D3C8,Q8DBX8,Q8DLK8,Q8EHC8,Q8EY44,Q8FL16,Q8FSD4,Q8KAQ7,Q8NT73,Q8NVU6,Q8NW75,Q8P5R4,Q8PH40,Q8PW58,Q8RFY7,Q8TT57,Q8TYL6,Q8X4V5,Q8Y1M4,Q8Y6J9,Q8Y6X8,Q8YS26,Q8Z9B4,Q8ZBL9,Q8ZYW1,Q92AX5,Q92BG1,Q976H2,Q97B25,Q97MU2,Q980U5,Q99T15,Q9CNG9,Q9F2S0,Q9HKM6,Q9HMY8,Q9JRW9,Q9JW10,Q9JXW0,Q9K8G3,Q9KEB0,Q9KU97,Q9PB43,Q9PKI3,Q9PP70,Q9RWW0,Q9Y9I9,Q9ZMD0</t>
+          <t xml:space="preserve">R02272: [] | GSAAMINOTRANS-RXN: [A0AJ02, A0AJD9, A0B885, A0JYM2, A0K5D7, A0KNY9, A0KZS6, A0L3S9, A0LIP3, A0LRE5, A0LXY3, A0PLS0, A0Q2A8, A0Q628, A0QLG2, A0QR33, A0R9G6, A0RJ78, A0RQ51, A0RXB3, A1A7K0, A1ASE9, A1AVQ1, A1BJG8, A1JJQ1, A1KB59, A1KG00, A1KS34, A1R898, A1RMG7, A1RQR5, A1S3U0, A1SE06, A1ST92, A1T3F2, A1TKK8, A1TYG5, A1UAR1, A1V1L0, A1V9X6, A1VSM6, A1VZJ6, A1WBR8, A1WMA0, A1WYL3, A2BL27, A2BPW6, A2BVE5, A2C0U2, A2C7I7, A2S9D9, A2SKQ7, A2SQU3, A3CL81, A3CU65, A3D1R5, A3DIF3, A3M7I8, A3MMQ8, A3MWW7, A3N2K3, A3NCF3, A3NY82, A3PBK8, A3PUB7, A3QBN5, A4FPX3, A4FZY1, A4G8N0, A4IKL1, A4IRG2, A4IXN8, A4J6H0, A4JC86, A4QB78, A4SGT2, A4SJ79, A4SVE6, A4T358, A4TPW6, A4VQY0, A4W6Q1, A4WN33, A4XC73, A4XK09, A4XYV6, A4Y4G4, A4YD91, A5CNI7, A5CXH8, A5D3M2, A5EXX1, A5F945, A5FIM3, A5G9C0, A5GMT2, A5GUJ2, A5IC29, A5ITJ2, A5IU30, A5N5Y1, A5TZQ4, A5UML0, A5UU40, A5VM65, A5W9H0, A5WC94, A6GYW4, A6LKX4, A6LSY8, A6Q2X6, A6Q9P9, A6QHK1, A6QI46, A6T2A2, A6T4V8, A6TJD8, A6U2D5, A6U2W8, A6URL2, A6UWB3, A6V0D2, A6VIL1, A6VQ66, A6VUX8, A6W5M6, A6WKL6, A7FM09, A7GL00, A7GTE2, A7GXK4, A7H3N1, A7HIX3, A7I252, A7I7P2, A7MGR5, A7MUU9, A7NCX8, A7NKV1, A7X388, A7X3X9, A7Z2N8, A7Z7A2, A7ZCH5, A7ZHP6, A7ZWA2, A8AAB3, A8ALD5, A8ETJ2, A8FB92, A8FFU9, A8FLR2, A8FS76, A8G3J9, A8G9U7, A8H164, A8LCD0, A8M6S5, A8M919, A8MGY8, A8YY36, A8Z2I8, A8ZZU9, A9A1A0, A9A875, A9AEU0, A9B550, A9BEA5, A9BY74, A9GDD3, A9I1R3, A9KBA0, A9KP86, A9KSC7, A9L5J5, A9M1G6, A9MPK7, A9N0P9, A9NAX3, A9R1E6, A9VIT5, A9VSS7, A9WIS7, A9WPI0, B0B9W0, B0BBJ0, B0BRF0, B0CC57, B0JPW6, B0KJV9, B0R7L9, B0RBL3, B0RP74, B0SF64, B0SNK3, B0TFV0, B0TIQ0, B0U0T6, B0U328, B0UST3, B0VCN6, B0VU92, B1HUT1, B1HVD3, B1I4L1, B1IQI6, B1J1Y6, B1JK22, B1JX81, B1KHF6, B1LGV7, B1MHH1, B1VEK3, B1VTD1, B1X023, B1XD24, B1XIT5, B1XT79, B1Y8G2, B1YBL3, B1YJU8, B1YK58, B1YUJ7, B1ZVF7, B2A1H4, B2FT35, B2G9H2, B2GL27, B2HRL5, B2HW19, B2I6C2, B2J7M9, B2JED5, B2K547, B2SGG7, B2SKS0, B2T6C2, B2TPD4, B2U2Z9, B2U6Q7, B2UNE3, B2USD7, B2UX41, B2V5U0, B2VE25, B3DY05, B3E9X0, B3EI07, B3EKJ7, B3GYN8, B3PL68, B3QRD2, B3QSA6, B3R312, B4EBT3, B4EUE1, B4RNX2, B4S0D0, B4S3Q6, B4SGW1, B4SI23, B4SUY4, B4TK30, B4TXQ6, B4U8M6, B4UKE6, B5BL82, B5EFG4, B5ERN9, B5F8R5, B5FAL8, B5FJ01, B5R3G6, B5RHE0, B5Y1L5, B5YHH6, B5Z0D4, B5ZA72, B6EL04, B6HZD0, B6J3H2, B6J495, B6JKN5, B7GH35, B7GIK0, B7GYZ5, B7H9S6, B7HE93, B7HQM1, B7HU66, B7I4N4, B7IHH3, B7IIX2, B7IW22, B7JBI1, B7JNG6, B7JQ54, B7K2I1, B7KA18, B7LGL6, B7LWB5, B7M195, B7MBD7, B7MP16, B7N823, B7NIB7, B7UIK1, B7V9D9, B7VJJ5, B8CJG4, B8DFN7, B8DHJ5, B8DN02, B8EBU3, B8F7H5, B8FBA1, B8G2L6, B8G822, B8GJJ2, B8GLE4, B8HBR2, B8HYK1, B8I0R1, B8J3A3, B8JCU6, B8ZT67, B9DMX3, B9DND8, B9DZG0, B9E740, B9E7Y3, B9IZ36, B9J3N2, B9KFS8, B9L0Q2, B9LA83, B9LKS0, B9LTZ9, B9LZL6, B9MF68, B9MRJ7, C0Q5R5, C0QCR9, C0QQ98, C0Z671, C0ZAH4, C0ZUX9, C1A7K7, C1AKK4, C1AZ30, C1CWI8, C1D9B6, C1DMY5, C1DUY4, C1ETQ7, C1EWG6, C1F911, C1KVK0, C1KVY4, C3K2K3, C3L6Z2, C3LHA0, C3LSN1, C3MJ22, C3MYE0, C3MZR9, C3N842, C3NF69, C3P9E6, C3PCZ3, C3PKI4, C4K6Y5, C4KJ00, C4L367, C4L4J9, C4LAK4, C4ZRP7, C5BAP9, C6AR33, C6DC32, E1W874, O26330, O29027, O66998, O74038, O74061, O84212, P0C1P8, P0C2D9, P0CL07, P18492, P21267, P23893, P24630, P30949, P31593, P45621, P46716, P48247, P56115, P63507, P63508, P71084, P99096, P9WMN8, P9WMN9, Q01YQ2, Q02SE5, Q04NV4, Q04X52, Q06741, Q06774, Q07YU5, Q0AAH7, Q0AFV1, Q0AZ36, Q0BHJ2, Q0BLC7, Q0HG53, Q0HSE6, Q0I3R7, Q0I8G1, Q0KDN9, Q0RS03, Q0SF42, Q0ST19, Q0T852, Q0TLH7, Q0TQG7, Q0VSP6, Q0W5T3, Q110Z9, Q11WK1, Q12EF7, Q12KC8, Q12WM7, Q13V40, Q14HS1, Q15YL3, Q17X40, Q18ES5, Q1AUK6, Q1BE73, Q1BYB1, Q1C3X1, Q1CLU7, Q1CUJ7, Q1DFA7, Q1GXW0, Q1I4H5, Q1IHV2, Q1IWZ8, Q1LQM3, Q1MPW7, Q1QEE8, Q1QSB0, Q1RG34, Q21MJ0, Q21YQ0, Q24VD4, Q254Z2, Q2A2U8, Q2FFN1, Q2FG69, Q2FTK5, Q2FXR4, Q2G283, Q2IHP8, Q2JFQ1, Q2JMP7, Q2JS70, Q2KUS4, Q2LVW6, Q2NF42, Q2NVQ0, Q2P6E4, Q2RJ31, Q2S1S3, Q2S8X9, Q2SYB2, Q2Y5Q5, Q2YTC2, Q2YU22, Q30RJ4, Q30WH2, Q31C50, Q31FB1, Q31QJ2, Q325Y5, Q32JV4, Q39566, Q39IQ4, Q39QA6, Q3A7W5, Q3ACS9, Q3ALU9, Q3AP59, Q3AWP4, Q3B1A1, Q3BPP7, Q3IHS1, Q3IT20, Q3JDH7, Q3JPN1, Q3K6C0, Q3KMF2, Q3M3B9, Q3SFU6, Q3Z5K3, Q40147, Q42522, Q46CH1, Q46GT9, Q46XZ7, Q478V1, Q47LB3, Q47V96, Q48DP1, Q49Y99, Q49YQ9, Q4FVC4, Q4JAM7, Q4JSY1, Q4K5I6, Q4L706, Q4L7G9, Q4UYA7, Q4ZNA0, Q55665, Q57T53, Q58020, Q5E2W6, Q5FAH9, Q5H3I5, Q5HER0, Q5HFA5, Q5HN71, Q5HNN6, Q5HUU3, Q5KWK9, Q5L2S4, Q5L5P0, Q5NGB9, Q5P6J6, Q5PD43, Q5QVP9, Q5SJS4, Q5UZ90, Q5WEP8, Q5WIE9, Q5WWG1, Q5X529, Q5YP79, Q5ZVA6, Q60CV0, Q62HV8, Q633Y3, Q63GB4, Q63RP8, Q65GK4, Q65M82, Q65U43, Q66EF1, Q67KM3, Q6AB08, Q6AHE8, Q6AQ32, Q6D1Z0, Q6FCY1, Q6G870, Q6G8Q8, Q6GFJ3, Q6GG38, Q6HD65, Q6HNS8, Q6L2G9, Q6LUS3, Q6M0P5, Q6MAC7, Q6MHT9, Q6NJJ2, Q6YZE2, Q71YY2, Q71ZB5, Q725I1, Q72K83, Q72ZW5, Q73DX4, Q73SQ3, Q74GA9, Q75G04, Q7A4T5, Q7M847, Q7MHY9, Q7N845, Q7NPI4, Q7P1Z5, Q7U598, Q7UPM9, Q7V2J3, Q7V677, Q7VDA1, Q7VHK3, Q7W050, Q7W3U1, Q7WF71, Q817R3, Q81I85, Q81LD0, Q81YV0, Q821C1, Q822Q0, Q82E21, Q82UQ8, Q83AK3, Q83FJ5, Q83H98, Q85WB7, Q87BW3, Q87LY3, Q87VY5, Q88DP0, Q897K4, Q8CNZ1, Q8CRW7, Q8CV56, Q8CZE3, Q8D3C8, Q8DBX8, Q8DLK8, Q8EHC8, Q8EY44, Q8FL16, Q8FSD4, Q8KAQ7, Q8NT73, Q8NVU6, Q8NW75, Q8P5R4, Q8PH40, Q8PW58, Q8RFY7, Q8TT57, Q8TYL6, Q8X4V5, Q8Y1M4, Q8Y6J9, Q8Y6X8, Q8YS26, Q8Z9B4, Q8ZBL9, Q8ZYW1, Q92AX5, Q92BG1, Q976H2, Q97B25, Q97MU2, Q980U5, Q99T15, Q9CNG9, Q9F2S0, Q9HKM6, Q9HMY8, Q9JRW9, Q9JW10, Q9JXW0, Q9K8G3, Q9KEB0, Q9KU97, Q9PB43, Q9PKI3, Q9PP70, Q9RWW0, Q9Y9I9, Q9ZMD0] | 5.4.3.8_1: [] | </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>A1ADQ1,A4YXN2,A5EGD7,A7ZPI2,A8A2M8,B1IX88,B1LMH0,B1X9P6,B2TWX3,B3QBS6,B5YYX4,B6I6S5,B6JE29,B7LBS7,B7M6P3,B7MH34,B7MY33,B7N5X4,B7NPQ8,B7UG84,C4ZVR1,O06644,O87838,P69902,P69903,Q07Q82,Q0TF87,Q139H7,Q1R8Z2,Q217M3,Q2IUI7,Q31Y97,Q32DG9,Q3YZF6,Q6N8F8,Q82M40,Q89QH2,Q8FFE8,Q8XBR7</t>
+          <t xml:space="preserve">RXN0-1382: [A1ADQ1, A4YXN2, A5EGD7, A7ZPI2, A8A2M8, B1IX88, B1LMH0, B1X9P6, B2TWX3, B3QBS6, B5YYX4, B6I6S5, B6JE29, B7LBS7, B7M6P3, B7MH34, B7MY33, B7N5X4, B7NPQ8, B7UG84, C4ZVR1, O06644, O87838, P69902, P69903, Q07Q82, Q0TF87, Q139H7, Q1R8Z2, Q217M3, Q2IUI7, Q31Y97, Q32DG9, Q3YZF6, Q6N8F8, Q82M40, Q89QH2, Q8FFE8, Q8XBR7] | R07290: [] | 2.8.3.16_1: [] | </t>
         </is>
       </c>
     </row>
@@ -822,15 +858,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Q88JX9</t>
+          <t xml:space="preserve">RXN-12074: [Q88JX9] | R00008_reverse: [] | 4.1.3.17_7: [] | 4.1.3.17-RXN: [] | </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A0AJ02,A0AJD9,A0B885,A0JYM2,A0K5D7,A0KNY9,A0KZS6,A0L3S9,A0LIP3,A0LRE5,A0LXY3,A0PLS0,A0Q2A8,A0Q628,A0QLG2,A0QR33,A0R9G6,A0RJ78,A0RQ51,A0RXB3,A1A7K0,A1ASE9,A1AVQ1,A1BJG8,A1JJQ1,A1KB59,A1KG00,A1KS34,A1R898,A1RMG7,A1RQR5,A1S3U0,A1SE06,A1ST92,A1T3F2,A1TKK8,A1TYG5,A1UAR1,A1V1L0,A1V9X6,A1VSM6,A1VZJ6,A1WBR8,A1WMA0,A1WYL3,A2BL27,A2BPW6,A2BVE5,A2C0U2,A2C7I7,A2S9D9,A2SKQ7,A2SQU3,A3CL81,A3CU65,A3D1R5,A3DIF3,A3M7I8,A3MMQ8,A3MWW7,A3N2K3,A3NCF3,A3NY82,A3PBK8,A3PUB7,A3QBN5,A4FPX3,A4FZY1,A4G8N0,A4IKL1,A4IRG2,A4IXN8,A4J6H0,A4JC86,A4QB78,A4SGT2,A4SJ79,A4SVE6,A4T358,A4TPW6,A4VQY0,A4W6Q1,A4WN33,A4XC73,A4XK09,A4XYV6,A4Y4G4,A4YD91,A5CNI7,A5CXH8,A5D3M2,A5EXX1,A5F945,A5FIM3,A5G9C0,A5GMT2,A5GUJ2,A5IC29,A5ITJ2,A5IU30,A5N5Y1,A5TZQ4,A5UML0,A5UU40,A5VM65,A5W9H0,A5WC94,A6GYW4,A6LKX4,A6LSY8,A6Q2X6,A6Q9P9,A6QHK1,A6QI46,A6T2A2,A6T4V8,A6TJD8,A6U2D5,A6U2W8,A6URL2,A6UWB3,A6V0D2,A6VIL1,A6VQ66,A6VUX8,A6W5M6,A6WKL6,A7FM09,A7GL00,A7GTE2,A7GXK4,A7H3N1,A7HIX3,A7I252,A7I7P2,A7MGR5,A7MUU9,A7NCX8,A7NKV1,A7X388,A7X3X9,A7Z2N8,A7Z7A2,A7ZCH5,A7ZHP6,A7ZWA2,A8AAB3,A8ALD5,A8ETJ2,A8FB92,A8FFU9,A8FLR2,A8FS76,A8G3J9,A8G9U7,A8H164,A8LCD0,A8M6S5,A8M919,A8MGY8,A8YY36,A8Z2I8,A8ZZU9,A9A1A0,A9A875,A9AEU0,A9B550,A9BEA5,A9BY74,A9GDD3,A9I1R3,A9KBA0,A9KP86,A9KSC7,A9L5J5,A9M1G6,A9MPK7,A9N0P9,A9NAX3,A9R1E6,A9VIT5,A9VSS7,A9WIS7,A9WPI0,B0B9W0,B0BBJ0,B0BRF0,B0CC57,B0JPW6,B0KJV9,B0R7L9,B0RBL3,B0RP74,B0SF64,B0SNK3,B0TFV0,B0TIQ0,B0U0T6,B0U328,B0UST3,B0VCN6,B0VU92,B1HUT1,B1HVD3,B1I4L1,B1IQI6,B1J1Y6,B1JK22,B1JX81,B1KHF6,B1LGV7,B1MHH1,B1VEK3,B1VTD1,B1X023,B1XD24,B1XIT5,B1XT79,B1Y8G2,B1YBL3,B1YJU8,B1YK58,B1YUJ7,B1ZVF7,B2A1H4,B2FT35,B2G9H2,B2GL27,B2HRL5,B2HW19,B2I6C2,B2J7M9,B2JED5,B2K547,B2SGG7,B2SKS0,B2T6C2,B2TPD4,B2U2Z9,B2U6Q7,B2UNE3,B2USD7,B2UX41,B2V5U0,B2VE25,B3DY05,B3E9X0,B3EI07,B3EKJ7,B3GYN8,B3PL68,B3QRD2,B3QSA6,B3R312,B4EBT3,B4EUE1,B4RNX2,B4S0D0,B4S3Q6,B4SGW1,B4SI23,B4SUY4,B4TK30,B4TXQ6,B4U8M6,B4UKE6,B5BL82,B5EFG4,B5ERN9,B5F8R5,B5FAL8,B5FJ01,B5R3G6,B5RHE0,B5Y1L5,B5YHH6,B5Z0D4,B5ZA72,B6EL04,B6HZD0,B6J3H2,B6J495,B6JKN5,B7GH35,B7GIK0,B7GYZ5,B7H9S6,B7HE93,B7HQM1,B7HU66,B7I4N4,B7IHH3,B7IIX2,B7IW22,B7JBI1,B7JNG6,B7JQ54,B7K2I1,B7KA18,B7LGL6,B7LWB5,B7M195,B7MBD7,B7MP16,B7N823,B7NIB7,B7UIK1,B7V9D9,B7VJJ5,B8CJG4,B8DFN7,B8DHJ5,B8DN02,B8EBU3,B8F7H5,B8FBA1,B8G2L6,B8G822,B8GJJ2,B8GLE4,B8HBR2,B8HYK1,B8I0R1,B8J3A3,B8JCU6,B8ZT67,B9DMX3,B9DND8,B9DZG0,B9E740,B9E7Y3,B9IZ36,B9J3N2,B9KFS8,B9L0Q2,B9LA83,B9LKS0,B9LTZ9,B9LZL6,B9MF68,B9MRJ7,C0Q5R5,C0QCR9,C0QQ98,C0Z671,C0ZAH4,C0ZUX9,C1A7K7,C1AKK4,C1AZ30,C1CWI8,C1D9B6,C1DMY5,C1DUY4,C1ETQ7,C1EWG6,C1F911,C1KVK0,C1KVY4,C3K2K3,C3L6Z2,C3LHA0,C3LSN1,C3MJ22,C3MYE0,C3MZR9,C3N842,C3NF69,C3P9E6,C3PCZ3,C3PKI4,C4K6Y5,C4KJ00,C4L367,C4L4J9,C4LAK4,C4ZRP7,C5BAP9,C6AR33,C6DC32,E1W874,O26330,O29027,O66998,O74038,O74061,O84212,P0C1P8,P0C2D9,P0CL07,P18492,P21267,P23893,P24630,P30949,P31593,P45621,P46716,P48247,P56115,P63507,P63508,P71084,P99096,P9WMN8,P9WMN9,Q01YQ2,Q02SE5,Q04NV4,Q04X52,Q06741,Q06774,Q07YU5,Q0AAH7,Q0AFV1,Q0AZ36,Q0BHJ2,Q0BLC7,Q0HG53,Q0HSE6,Q0I3R7,Q0I8G1,Q0KDN9,Q0RS03,Q0SF42,Q0ST19,Q0T852,Q0TLH7,Q0TQG7,Q0VSP6,Q0W5T3,Q110Z9,Q11WK1,Q12EF7,Q12KC8,Q12WM7,Q13V40,Q14HS1,Q15YL3,Q17X40,Q18ES5,Q1AUK6,Q1BE73,Q1BYB1,Q1C3X1,Q1CLU7,Q1CUJ7,Q1DFA7,Q1GXW0,Q1I4H5,Q1IHV2,Q1IWZ8,Q1LQM3,Q1MPW7,Q1QEE8,Q1QSB0,Q1RG34,Q21MJ0,Q21YQ0,Q24VD4,Q254Z2,Q2A2U8,Q2FFN1,Q2FG69,Q2FTK5,Q2FXR4,Q2G283,Q2IHP8,Q2JFQ1,Q2JMP7,Q2JS70,Q2KUS4,Q2LVW6,Q2NF42,Q2NVQ0,Q2P6E4,Q2RJ31,Q2S1S3,Q2S8X9,Q2SYB2,Q2Y5Q5,Q2YTC2,Q2YU22,Q30RJ4,Q30WH2,Q31C50,Q31FB1,Q31QJ2,Q325Y5,Q32JV4,Q39566,Q39IQ4,Q39QA6,Q3A7W5,Q3ACS9,Q3ALU9,Q3AP59,Q3AWP4,Q3B1A1,Q3BPP7,Q3IHS1,Q3IT20,Q3JDH7,Q3JPN1,Q3K6C0,Q3KMF2,Q3M3B9,Q3SFU6,Q3Z5K3,Q40147,Q42522,Q46CH1,Q46GT9,Q46XZ7,Q478V1,Q47LB3,Q47V96,Q48DP1,Q49Y99,Q49YQ9,Q4FVC4,Q4JAM7,Q4JSY1,Q4K5I6,Q4L706,Q4L7G9,Q4UYA7,Q4ZNA0,Q55665,Q57T53,Q58020,Q5E2W6,Q5FAH9,Q5H3I5,Q5HER0,Q5HFA5,Q5HN71,Q5HNN6,Q5HUU3,Q5KWK9,Q5L2S4,Q5L5P0,Q5NGB9,Q5P6J6,Q5PD43,Q5QVP9,Q5SJS4,Q5UZ90,Q5WEP8,Q5WIE9,Q5WWG1,Q5X529,Q5YP79,Q5ZVA6,Q60CV0,Q62HV8,Q633Y3,Q63GB4,Q63RP8,Q65GK4,Q65M82,Q65U43,Q66EF1,Q67KM3,Q6AB08,Q6AHE8,Q6AQ32,Q6D1Z0,Q6FCY1,Q6G870,Q6G8Q8,Q6GFJ3,Q6GG38,Q6HD65,Q6HNS8,Q6L2G9,Q6LUS3,Q6M0P5,Q6MAC7,Q6MHT9,Q6NJJ2,Q6YZE2,Q71YY2,Q71ZB5,Q725I1,Q72K83,Q72ZW5,Q73DX4,Q73SQ3,Q74GA9,Q75G04,Q7A4T5,Q7M847,Q7MHY9,Q7N845,Q7NPI4,Q7P1Z5,Q7U598,Q7UPM9,Q7V2J3,Q7V677,Q7VDA1,Q7VHK3,Q7W050,Q7W3U1,Q7WF71,Q817R3,Q81I85,Q81LD0,Q81YV0,Q821C1,Q822Q0,Q82E21,Q82UQ8,Q83AK3,Q83FJ5,Q83H98,Q85WB7,Q87BW3,Q87LY3,Q87VY5,Q88DP0,Q897K4,Q8CNZ1,Q8CRW7,Q8CV56,Q8CZE3,Q8D3C8,Q8DBX8,Q8DLK8,Q8EHC8,Q8EY44,Q8FL16,Q8FSD4,Q8KAQ7,Q8NT73,Q8NVU6,Q8NW75,Q8P5R4,Q8PH40,Q8PW58,Q8RFY7,Q8TT57,Q8TYL6,Q8X4V5,Q8Y1M4,Q8Y6J9,Q8Y6X8,Q8YS26,Q8Z9B4,Q8ZBL9,Q8ZYW1,Q92AX5,Q92BG1,Q976H2,Q97B25,Q97MU2,Q980U5,Q99T15,Q9CNG9,Q9F2S0,Q9HKM6,Q9HMY8,Q9JRW9,Q9JW10,Q9JXW0,Q9K8G3,Q9KEB0,Q9KU97,Q9PB43,Q9PKI3,Q9PP70,Q9RWW0,Q9Y9I9,Q9ZMD0</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t xml:space="preserve">R02272: [] | GSAAMINOTRANS-RXN: [A0AJ02, A0AJD9, A0B885, A0JYM2, A0K5D7, A0KNY9, A0KZS6, A0L3S9, A0LIP3, A0LRE5, A0LXY3, A0PLS0, A0Q2A8, A0Q628, A0QLG2, A0QR33, A0R9G6, A0RJ78, A0RQ51, A0RXB3, A1A7K0, A1ASE9, A1AVQ1, A1BJG8, A1JJQ1, A1KB59, A1KG00, A1KS34, A1R898, A1RMG7, A1RQR5, A1S3U0, A1SE06, A1ST92, A1T3F2, A1TKK8, A1TYG5, A1UAR1, A1V1L0, A1V9X6, A1VSM6, A1VZJ6, A1WBR8, A1WMA0, A1WYL3, A2BL27, A2BPW6, A2BVE5, A2C0U2, A2C7I7, A2S9D9, A2SKQ7, A2SQU3, A3CL81, A3CU65, A3D1R5, A3DIF3, A3M7I8, A3MMQ8, A3MWW7, A3N2K3, A3NCF3, A3NY82, A3PBK8, A3PUB7, A3QBN5, A4FPX3, A4FZY1, A4G8N0, A4IKL1, A4IRG2, A4IXN8, A4J6H0, A4JC86, A4QB78, A4SGT2, A4SJ79, A4SVE6, A4T358, A4TPW6, A4VQY0, A4W6Q1, A4WN33, A4XC73, A4XK09, A4XYV6, A4Y4G4, A4YD91, A5CNI7, A5CXH8, A5D3M2, A5EXX1, A5F945, A5FIM3, A5G9C0, A5GMT2, A5GUJ2, A5IC29, A5ITJ2, A5IU30, A5N5Y1, A5TZQ4, A5UML0, A5UU40, A5VM65, A5W9H0, A5WC94, A6GYW4, A6LKX4, A6LSY8, A6Q2X6, A6Q9P9, A6QHK1, A6QI46, A6T2A2, A6T4V8, A6TJD8, A6U2D5, A6U2W8, A6URL2, A6UWB3, A6V0D2, A6VIL1, A6VQ66, A6VUX8, A6W5M6, A6WKL6, A7FM09, A7GL00, A7GTE2, A7GXK4, A7H3N1, A7HIX3, A7I252, A7I7P2, A7MGR5, A7MUU9, A7NCX8, A7NKV1, A7X388, A7X3X9, A7Z2N8, A7Z7A2, A7ZCH5, A7ZHP6, A7ZWA2, A8AAB3, A8ALD5, A8ETJ2, A8FB92, A8FFU9, A8FLR2, A8FS76, A8G3J9, A8G9U7, A8H164, A8LCD0, A8M6S5, A8M919, A8MGY8, A8YY36, A8Z2I8, A8ZZU9, A9A1A0, A9A875, A9AEU0, A9B550, A9BEA5, A9BY74, A9GDD3, A9I1R3, A9KBA0, A9KP86, A9KSC7, A9L5J5, A9M1G6, A9MPK7, A9N0P9, A9NAX3, A9R1E6, A9VIT5, A9VSS7, A9WIS7, A9WPI0, B0B9W0, B0BBJ0, B0BRF0, B0CC57, B0JPW6, B0KJV9, B0R7L9, B0RBL3, B0RP74, B0SF64, B0SNK3, B0TFV0, B0TIQ0, B0U0T6, B0U328, B0UST3, B0VCN6, B0VU92, B1HUT1, B1HVD3, B1I4L1, B1IQI6, B1J1Y6, B1JK22, B1JX81, B1KHF6, B1LGV7, B1MHH1, B1VEK3, B1VTD1, B1X023, B1XD24, B1XIT5, B1XT79, B1Y8G2, B1YBL3, B1YJU8, B1YK58, B1YUJ7, B1ZVF7, B2A1H4, B2FT35, B2G9H2, B2GL27, B2HRL5, B2HW19, B2I6C2, B2J7M9, B2JED5, B2K547, B2SGG7, B2SKS0, B2T6C2, B2TPD4, B2U2Z9, B2U6Q7, B2UNE3, B2USD7, B2UX41, B2V5U0, B2VE25, B3DY05, B3E9X0, B3EI07, B3EKJ7, B3GYN8, B3PL68, B3QRD2, B3QSA6, B3R312, B4EBT3, B4EUE1, B4RNX2, B4S0D0, B4S3Q6, B4SGW1, B4SI23, B4SUY4, B4TK30, B4TXQ6, B4U8M6, B4UKE6, B5BL82, B5EFG4, B5ERN9, B5F8R5, B5FAL8, B5FJ01, B5R3G6, B5RHE0, B5Y1L5, B5YHH6, B5Z0D4, B5ZA72, B6EL04, B6HZD0, B6J3H2, B6J495, B6JKN5, B7GH35, B7GIK0, B7GYZ5, B7H9S6, B7HE93, B7HQM1, B7HU66, B7I4N4, B7IHH3, B7IIX2, B7IW22, B7JBI1, B7JNG6, B7JQ54, B7K2I1, B7KA18, B7LGL6, B7LWB5, B7M195, B7MBD7, B7MP16, B7N823, B7NIB7, B7UIK1, B7V9D9, B7VJJ5, B8CJG4, B8DFN7, B8DHJ5, B8DN02, B8EBU3, B8F7H5, B8FBA1, B8G2L6, B8G822, B8GJJ2, B8GLE4, B8HBR2, B8HYK1, B8I0R1, B8J3A3, B8JCU6, B8ZT67, B9DMX3, B9DND8, B9DZG0, B9E740, B9E7Y3, B9IZ36, B9J3N2, B9KFS8, B9L0Q2, B9LA83, B9LKS0, B9LTZ9, B9LZL6, B9MF68, B9MRJ7, C0Q5R5, C0QCR9, C0QQ98, C0Z671, C0ZAH4, C0ZUX9, C1A7K7, C1AKK4, C1AZ30, C1CWI8, C1D9B6, C1DMY5, C1DUY4, C1ETQ7, C1EWG6, C1F911, C1KVK0, C1KVY4, C3K2K3, C3L6Z2, C3LHA0, C3LSN1, C3MJ22, C3MYE0, C3MZR9, C3N842, C3NF69, C3P9E6, C3PCZ3, C3PKI4, C4K6Y5, C4KJ00, C4L367, C4L4J9, C4LAK4, C4ZRP7, C5BAP9, C6AR33, C6DC32, E1W874, O26330, O29027, O66998, O74038, O74061, O84212, P0C1P8, P0C2D9, P0CL07, P18492, P21267, P23893, P24630, P30949, P31593, P45621, P46716, P48247, P56115, P63507, P63508, P71084, P99096, P9WMN8, P9WMN9, Q01YQ2, Q02SE5, Q04NV4, Q04X52, Q06741, Q06774, Q07YU5, Q0AAH7, Q0AFV1, Q0AZ36, Q0BHJ2, Q0BLC7, Q0HG53, Q0HSE6, Q0I3R7, Q0I8G1, Q0KDN9, Q0RS03, Q0SF42, Q0ST19, Q0T852, Q0TLH7, Q0TQG7, Q0VSP6, Q0W5T3, Q110Z9, Q11WK1, Q12EF7, Q12KC8, Q12WM7, Q13V40, Q14HS1, Q15YL3, Q17X40, Q18ES5, Q1AUK6, Q1BE73, Q1BYB1, Q1C3X1, Q1CLU7, Q1CUJ7, Q1DFA7, Q1GXW0, Q1I4H5, Q1IHV2, Q1IWZ8, Q1LQM3, Q1MPW7, Q1QEE8, Q1QSB0, Q1RG34, Q21MJ0, Q21YQ0, Q24VD4, Q254Z2, Q2A2U8, Q2FFN1, Q2FG69, Q2FTK5, Q2FXR4, Q2G283, Q2IHP8, Q2JFQ1, Q2JMP7, Q2JS70, Q2KUS4, Q2LVW6, Q2NF42, Q2NVQ0, Q2P6E4, Q2RJ31, Q2S1S3, Q2S8X9, Q2SYB2, Q2Y5Q5, Q2YTC2, Q2YU22, Q30RJ4, Q30WH2, Q31C50, Q31FB1, Q31QJ2, Q325Y5, Q32JV4, Q39566, Q39IQ4, Q39QA6, Q3A7W5, Q3ACS9, Q3ALU9, Q3AP59, Q3AWP4, Q3B1A1, Q3BPP7, Q3IHS1, Q3IT20, Q3JDH7, Q3JPN1, Q3K6C0, Q3KMF2, Q3M3B9, Q3SFU6, Q3Z5K3, Q40147, Q42522, Q46CH1, Q46GT9, Q46XZ7, Q478V1, Q47LB3, Q47V96, Q48DP1, Q49Y99, Q49YQ9, Q4FVC4, Q4JAM7, Q4JSY1, Q4K5I6, Q4L706, Q4L7G9, Q4UYA7, Q4ZNA0, Q55665, Q57T53, Q58020, Q5E2W6, Q5FAH9, Q5H3I5, Q5HER0, Q5HFA5, Q5HN71, Q5HNN6, Q5HUU3, Q5KWK9, Q5L2S4, Q5L5P0, Q5NGB9, Q5P6J6, Q5PD43, Q5QVP9, Q5SJS4, Q5UZ90, Q5WEP8, Q5WIE9, Q5WWG1, Q5X529, Q5YP79, Q5ZVA6, Q60CV0, Q62HV8, Q633Y3, Q63GB4, Q63RP8, Q65GK4, Q65M82, Q65U43, Q66EF1, Q67KM3, Q6AB08, Q6AHE8, Q6AQ32, Q6D1Z0, Q6FCY1, Q6G870, Q6G8Q8, Q6GFJ3, Q6GG38, Q6HD65, Q6HNS8, Q6L2G9, Q6LUS3, Q6M0P5, Q6MAC7, Q6MHT9, Q6NJJ2, Q6YZE2, Q71YY2, Q71ZB5, Q725I1, Q72K83, Q72ZW5, Q73DX4, Q73SQ3, Q74GA9, Q75G04, Q7A4T5, Q7M847, Q7MHY9, Q7N845, Q7NPI4, Q7P1Z5, Q7U598, Q7UPM9, Q7V2J3, Q7V677, Q7VDA1, Q7VHK3, Q7W050, Q7W3U1, Q7WF71, Q817R3, Q81I85, Q81LD0, Q81YV0, Q821C1, Q822Q0, Q82E21, Q82UQ8, Q83AK3, Q83FJ5, Q83H98, Q85WB7, Q87BW3, Q87LY3, Q87VY5, Q88DP0, Q897K4, Q8CNZ1, Q8CRW7, Q8CV56, Q8CZE3, Q8D3C8, Q8DBX8, Q8DLK8, Q8EHC8, Q8EY44, Q8FL16, Q8FSD4, Q8KAQ7, Q8NT73, Q8NVU6, Q8NW75, Q8P5R4, Q8PH40, Q8PW58, Q8RFY7, Q8TT57, Q8TYL6, Q8X4V5, Q8Y1M4, Q8Y6J9, Q8Y6X8, Q8YS26, Q8Z9B4, Q8ZBL9, Q8ZYW1, Q92AX5, Q92BG1, Q976H2, Q97B25, Q97MU2, Q980U5, Q99T15, Q9CNG9, Q9F2S0, Q9HKM6, Q9HMY8, Q9JRW9, Q9JW10, Q9JXW0, Q9K8G3, Q9KEB0, Q9KU97, Q9PB43, Q9PKI3, Q9PP70, Q9RWW0, Q9Y9I9, Q9ZMD0] | 5.4.3.8_1: [] | </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4.1.1.4_1: [] | </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Processed hopa and mvacid expansions for March bottle checkin
</commit_message>
<xml_diff>
--- a/artifacts/pwy_xls/ccm_v0_to_hopa_gen_3_tan_sample_1_n_samples_1000.xlsx
+++ b/artifacts/pwy_xls/ccm_v0_to_hopa_gen_3_tan_sample_1_n_samples_1000.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pyruvate_hopa" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="oxaloacetate_hopa" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="succinate_hopa" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="malate_hopa" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="oxaloacetate_hopa" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pyruvate_hopa" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,11 +495,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -508,43 +508,43 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>58.23487147501859</v>
+        <v>26.56969255872742</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5972222222222222</v>
+        <v>0.6791310541310541</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4540598290598291</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.8055555555555555</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>D5FKJ3</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Q643C8</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>G8FRC5</t>
+          <t>A0QTU8</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -553,43 +553,43 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>32.04739186446719</v>
+        <v>22.10950460088475</v>
       </c>
       <c r="E3" t="n">
+        <v>0.5731481481481481</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.5416666666666666</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.3333333333333333</v>
-      </c>
       <c r="H3" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.4</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Q88JX9, A5W059</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>E3PY96, E3PY95</t>
+          <t>Q643C8</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Q588Z2</t>
+          <t>Q59268</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -598,43 +598,43 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7.90381435109191</v>
+        <v>24.24741408404559</v>
       </c>
       <c r="E4" t="n">
-        <v>0.351010101010101</v>
+        <v>0.568097643097643</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.7626262626262625</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1363636363636364</v>
+        <v>0.4</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Q88JX9, A5W059</t>
+          <t>D5FKJ3</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>E3PY96, E3PY95</t>
+          <t>P00815</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>P0C017, O28997, P21264, P55195, P50504, Q01930, P15567, P22234, P0CQ36, Q73PV9, Q9UVE6, O74197, O80937, P0CQ37, Q92210</t>
+          <t>Q59268</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -643,43 +643,43 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>8.492132758669902</v>
+        <v>23.1305084350496</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3285353535353536</v>
+        <v>0.3282652532652533</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.1101010101010101</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="H5" t="n">
-        <v>0.06893939393939394</v>
+        <v>0.1524725274725275</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Q88JX9, A5W059</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>E3PY96, E3PY95</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -688,43 +688,43 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>11.89198569708731</v>
+        <v>25.57226975355714</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3285353535353536</v>
+        <v>0.5393458393458394</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.1101010101010101</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="H6" t="n">
-        <v>0.06893939393939394</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Q88JX9, A5W059</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>E3PY96, E3PY95</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q05957</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -733,43 +733,43 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>18.42954643354551</v>
+        <v>24.35179694036886</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3392255892255893</v>
+        <v>0.3369773744773745</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1287878787878788</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.08068181818181819</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.1524725274725275</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>A0A0H2WVX4, P31116, D8WXQ1, P08499, Q5AIA2, D8WXQ2, Q56R01, P46806, Q3S3F6, O81852</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>B8EBU3, B8GLE4, C5BAP9, A5F945, Q66EF1, B3E9X0, B0RP74, Q0T852, A4Y4G4, A1KG00, A6LSY8, A6Q9P9, Q8KAQ7, A8FFU9, B0U328, B9LZL6, A9N0P9, Q2G283, Q0SF42, Q15YL3, B3QRD2, C3K2K3, P71084, Q72K83, A9KSC7, Q32JV4, B8GJJ2, Q2FTK5, Q6GFJ3, A3PUB7, B1J1Y6, Q87LY3, C3L6Z2, B7UIK1, A8FLR2, A3DIF3, A7ZHP6, A7Z7A2, P0C2D9, Q9JRW9, B3QSA6, Q2A2U8, Q5PD43, A6UWB3, C0ZUX9, A2SQU3, O74061, A4IRG2, P0C1P8, P0CL07, A3MWW7, A4XC73, Q1LQM3, Q3AP59, Q3ACS9, A9GDD3, A5CNI7, Q8Y6J9, Q81I85, Q6HD65, A6TJD8, A6Q2X6, Q4FVC4, A4IKL1, B1JK22, Q0ST19, Q8FSD4, Q9PKI3, B9DZG0, Q976H2, A9VSS7, Q7VDA1, B2SGG7, B1HUT1, B1YK58, A1RQR5, Q4L706, A3N2K3, B4RNX2, Q07YU5, Q1QSB0, Q2S8X9, Q3JPN1, C1ETQ7, B8F7H5, B7GIK0, Q5FAH9, A9KP86, A5IC29, Q4L7G9, Q3AWP4, B1YUJ7, Q7WF71, A5EXX1, Q5P6J6, Q3A7W5, C4L4J9, A0R9G6, A6QHK1, B8HBR2, Q6FCY1, Q75G04, Q6G870, Q9K8G3, Q7V2J3, A7H3N1, Q6AHE8, Q1CUJ7, Q31FB1, B7N823, Q1DFA7, Q6AQ32, A6VUX8, P18492, P48247, A0KNY9, A7MGR5, A9WPI0, Q1GXW0, Q7MHY9, B7HU66, Q06741, B4SGW1, B0JPW6, P56115, Q0AAH7, C6AR33, A5W9H0, A5IU30, B7MBD7, P23893, Q4K5I6, B0UST3, Q2SYB2, B7H9S6, A5GUJ2, C1A7K7, A3NCF3, A1ST92, A8YY36, Q18ES5, A3MMQ8, Q5HUU3, A8G9U7, Q7P1Z5, Q8TYL6, B2TPD4, A8M6S5, A1SE06, B2J7M9, A1BJG8, B5Y1L5, Q8EHC8, A4SGT2, Q60CV0, B8CJG4, B3DY05, Q254Z2, Q6HNS8, B0VU92, Q725I1, B4EUE1, Q92AX5, A1V9X6, B4EBT3, C4LAK4, Q7V677, Q8X4V5, B0TIQ0, Q71ZB5, B9KFS8, Q5SJS4, B7IW22, Q88DP0, A5D3M2, B1MHH1, A2BL27, Q2JMP7, A0LIP3, B1LGV7, O26330, A1S3U0, Q46GT9, C3LSN1, Q63RP8, B2GL27, Q8NW75, Q49YQ9, B9LKS0, C1CWI8, B0SF64, B3PL68, A8M919, Q71YY2, Q14HS1, A1VSM6, A1ASE9, Q1MPW7, B2USD7, B1JX81, B2A1H4, A4T358, A6WKL6, P46716, A3CU65, P63508, O74038, Q40147, Q8EY44, B5BL82, Q8PH40, Q3ALU9, A5ITJ2, B4S0D0, Q73SQ3, A0LXY3, A4XK09, B0TFV0, Q92BG1, B9LA83, A1R898, B4TK30, Q12EF7, C0ZAH4, Q4JAM7, Q17X40, A1TYG5, Q2YU22, Q8ZYW1, A8ETJ2, O84212, B8HYK1, B2K547, Q6AB08, A2C0U2, Q24VD4, Q39566, Q83FJ5, Q9Y9I9, Q2JFQ1, A8H164, B1XD24, B1XIT5, B2U2Z9, B7V9D9, Q21YQ0, Q46CH1, P42799, Q30WH2, Q4ZNA0, Q0HG53, Q9HKM6, Q7N845, Q2NVQ0, B9IZ36, A0RXB3, Q0BHJ2, A4G8N0, B7NIB7, A7X3X9, Q3IHS1, C1AKK4, Q0W5T3, Q83AK3, Q06774, A4XYV6, B1Y8G2, C4KJ00, A0K5D7, A4FZY1, Q2FXR4, Q8CV56, A4TPW6, A5N5Y1, Q46XZ7, Q9ZMD0, Q3B1A1, Q48DP1, Q72ZW5, A2BPW6, B0SNK3, B5ERN9, Q6L2G9, Q81YV0, Q8DBX8, Q85WB7, B8G2L6, A9WIS7, B8ZT67, C0QCR9, A3NY82, Q7W050, Q3BPP7, B0B9W0, A4IXN8, B7MP16, Q5L2S4, P9WMN8, Q7VHK3, B3GYN8, A9NAX3, B1KHF6, Q4JSY1, A0PLS0, B3EKJ7, Q9F2S0, A1RMG7, B8J3A3, Q73DX4, A8LCD0, P45621, A8G3J9, A3QBN5, Q47LB3, A7HIX3, A7NCX8, Q97MU2, C1DMY5, A6V0D2, B2FT35, C4ZRP7, B7IHH3, B8DN02, B5Z0D4, A6URL2, A7MUU9, B9L0Q2, B9MRJ7, Q3IT20, Q2IHP8, P9WMN9, A1UAR1, C3PKI4, B7JQ54, B5EFG4, Q0BLC7, A5G9C0, B1YJU8, Q6NJJ2, Q817R3, A6W5M6, P30949, Q1CLU7, Q63GB4, Q821C1, B4S3Q6, B2SKS0, Q83H98, A6VQ66, B0CC57, Q8CRW7, E1W874, B1IQI6, Q0I3R7, Q3SFU6, Q478V1, B3EI07, Q13V40, Q2Y5Q5, B7VJJ5, Q47V96, B9J3N2, A5WC94, Q3M3B9, A7Z2N8, Q42522, B1X023, B1ZVF7, A1A7K0, B9DND8, A8ALD5, B8DHJ5, B7K2I1, Q1AUK6, C3LHA0, P24630, Q5HFA5, A4WN33, A8Z2I8, A2C7I7, A7GTE2, Q11WK1, B1YBL3, A1JJQ1, Q2S1S3, B7M195, A4VQY0, A4YD91, A5GMT2, B2HRL5, Q6G8Q8, Q04NV4, A3CL81, Q57T53, Q2NF42, Q2YTC2, Q8PW58, A7ZWA2, Q31C50, C0Q5R5, B7GH35, B7LWB5, B2HW19, C1DUY4, Q8D3C8, Q0AFV1, B2I6C2, Q6MAC7, P31593, Q2JS70, Q8CZE3, B9DMX3, Q8Z9B4, A4W6Q1, B9E740, C3MJ22, B5YHH6, A1TKK8, C3PCZ3, Q01YQ2, A0Q628, Q6LUS3, A2S9D9, A3M7I8, B1VEK3, Q6MHT9, Q3JDH7, Q9KEB0, B2T6C2, B8G822, C3NF69, B7IIX2, Q1I4H5, B4SUY4, A7FM09, Q65GK4, B7JNG6, Q2FG69, A9VIT5, Q5WEP8, A4QB78, Q1BYB1, A8ZZU9, A1AVQ1, A1V1L0, A0RQ51, B5R3G6, Q6M0P5, B2UNE3, B6HZD0, Q67KM3, A8FS76, C1EWG6, Q87VY5, Q7UPM9, Q12KC8, Q58020, A9R1E6, Q55665, Q5HNN6, B2JED5, Q8P5R4, B9LTZ9, A9M1G6, A2SKQ7, Q82E21, Q5ZVA6, A0B885, C3MZR9, Q897K4, Q5X529, Q1QEE8, A7I7P2, Q31QJ2, Q39IQ4, A7I252, C4L367, B4U8M6, A5TZQ4, B7HE93, Q2P6E4, B2U6Q7, B8I0R1, Q980U5, A9BY74, B7LGL6, Q0VSP6, C6DC32, Q8DLK8, B1HVD3, Q0TQG7, B7JBI1, A6GYW4, B4TXQ6, Q3Z5K3, Q9PP70, Q1IWZ8, A5VM65, A6T2A2, B9MF68, Q8FL16, Q0AZ36, B0BBJ0, A7ZCH5, B5FAL8, Q1BE73, B5F8R5, C1KVY4, Q5HER0, A1KS34, A8MGY8, B5RHE0, A6U2W8, A2BVE5, Q0RS03, B5FJ01, B7GYZ5, B8DFN7, A1WYL3, Q8TT57, B6EL04, B2V5U0, C0Z671, Q39QA6, Q0KDN9, Q0TLH7, A1VZJ6, B6J3H2, Q1RG34, B0VCN6, Q8CNZ1, Q9PB43, Q04X52, B1VTD1, Q2KUS4, B0BRF0, Q5H3I5, B8FBA1, Q9RWW0, Q5HN71, Q0I8G1, Q7NPI4, B1I4L1, Q1IHV2, Q74GA9, A6QI46, B7I4N4, A7GL00, B1XT79, Q7W3U1, B0U0T6, A0JYM2, Q633Y3, B4SI23, B0R7L9, A3D1R5, A0LRE5, Q6YZE2, Q7A4T5, Q49Y99, C1D9B6, O66998, Q1C3X1, A9A1A0, C1F911, A5FIM3, A1KB59, Q5L5P0, A1WMA0, A6VIL1, A1T3F2, A5CXH8, A0L3S9, Q5KWK9, A6U2D5, Q8YS26, A4SVE6, P63507, Q9JW10, A9BEA5, Q87BW3, B5ZA72, Q97B25, B2G9H2, Q110Z9, Q5YP79, Q9KU97, Q5WIE9, B7HQM1, B0KJV9, A7GXK4, Q6D1Z0, A9I1R3, Q12WM7, B3R312, Q5E2W6, A9A875, A0QR33, A9KBA0, A0QLG2, B6J495, Q5QVP9, A8AAB3, C1KVK0, Q5WWG1, Q99T15, A1WBR8, C3P9E6, Q8RFY7, A5UML0, Q5NGB9, Q5UZ90, Q0HSE6, Q4UYA7, Q8ZBL9, B7KA18, A7X388, Q8Y6X8, Q8NT73, Q21MJ0, Q2LVW6, B2UX41, B9E7Y3, Q325Y5, A8FB92, A5UU40, Q2RJ31, C1AZ30, Q3K6C0, Q62HV8, C4K6Y5, Q6GG38, A0Q2A8, Q822Q0, A7NKV1, Q7M847, A0AJD9, Q65M82, Q9JXW0, A4SJ79, Q30RJ4, O29027, Q9CNG9, Q82UQ8, Q65U43, Q8Y1M4, A3PBK8, C3MYE0, A9MPK7, A4J6H0, P99096, Q2FFN1, A4JC86, A6LKX4, Q9HMY8, A0RJ78, A9AEU0, C3N842, Q8NVU6, A4FPX3, B4UKE6, B6JKN5, C0QQ98, A9B550, Q7U598, A0KZS6, A6T4V8, Q3KMF2, A0AJ02, B8JCU6, B0RBL3, Q81LD0, Q02SE5, A9L5J5, B2VE25</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -778,43 +778,43 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>15.85866290964453</v>
+        <v>21.91006321265886</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.5480579605579605</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.08068181818181819</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Q9KJF0</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>G8FRC5</t>
+          <t>Q05957</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -823,43 +823,43 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>11.89198569423518</v>
+        <v>29.73474970552454</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2572150072150072</v>
+        <v>0.3101791726791727</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1287878787878788</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6428571428571428</v>
+        <v>0.08068181818181819</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.07207792207792207</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Q87C38, Q7PS09, Q2UUH5, C1BYA3, Q60AP7, C5D7V1, A6RI12, B8NSW2, Q5FW37, B0SU49, Q81MJ0, Q04WK2, Q0VPK5, Q8EXC1, Q3KFI9, A1TZ34, B7HN16, C1EQR3, B0U3A4, B5XZV4, A6V7A8, Q6CMZ9, Q96GX9, A3LVM9, B2I5X2, A9R2Z8, C1BJB1, C5JIC2, Q9VY93, C7GKY0, B2WCB2, A1JP13, B0Y4N9, Q3IJW1, C6H2R1, A7RH72, B0RSM5, A7TET7, A4W7Z4, Q0BPT9, D2VN51, B3MW09, C1DHH0, Q5AG73, Q2SKZ2, A5EES6, C5PIC1, B2SM82, B5X277, B4R4E9, A1CW59, B7IWF0, C4YRG6, A8GAA8, B0CZ32, B0SII1, P47095, C4XXU2, A2Q9M4, Q48KM8, Q6D1G1, A6T663, C1C4M8, Q02KH3, A7HU86, B3S866, Q16NX0, A7Z3X6, Q9HE08, Q6NU29, D1ZJC1, A6RAS3, Q4ZVC0, B4M1W5, A7GS62, Q04NC3, Q23261, C0S4Z7, B2VAA6, C0QSI8, Q29HV4, Q6CBB0, C6DCZ4, C5FEJ4, Q75FG3, A4TPN2, B1YIY0, B9WHK1, Q819E6, C5GGA4, B7H929, A7FLL4, A5DHV9, B4STR2, B8LXM1, B4L8M2, A8FCH0, P0CM14, Q0UUN6, B7JL18, Q4WQH4, Q8P9N3, Q635P1, Q3BUE6, A6ZPY9, A9H8G1, Q5ZLP2, A5E3E3, Q3ZUZ8, Q4Q882, B2FPP4, P0CM15, Q731R0, B4Q2F5, Q2NWC8, Q66E19, A9VCQ2, Q9WVQ5, Q5L1E0, A5FUG4, A4ILL7, B1JIK6, Q6BIX5, Q66I75, C4WU37, C5DCA2, B6K0X1, Q8PLG0, Q4UU51, A9FCX7, C4JKS2, C0NN25, C1G3Q0, C3P747, Q75CP5, Q9I342, A4RK52, O67788, Q7SF46, B4NEU3, B9IWQ1, C1H861, B4JLL3, B6HNY8, Q5H0X8, A8ANI0, Q6FJA5, B2K630, Q0CT19, Q5FRJ3, A7MK09, B6QQ13, Q9PBD5, Q5B787, A4HGN7, Q2HE69, A7EH92, C7YHA8, C4R7D9, Q2P3W4, Q884P3, C5MHJ2, A8NQV9, A0RI44, C3LIA8, A4I3R0, I7MAL0, B2A8X1, B3LQB9, C4KZ52, O31668, B7UV38, B4IG61, Q6HEC7, B5VLI6, B4GY79, B3NVZ7, A9VFE1, B0JVQ9, C5E0B9, B1XPT3, Q0VCJ2, A1CIK4</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Q1KLK1, Q1KLK0, A9WC40</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -868,43 +868,43 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>11.05256270781175</v>
+        <v>24.36708975704198</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.3101791726791727</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.08068181818181819</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.07207792207792207</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Q88JX9, A5W059</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Q588Z2</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>B8EBU3, B8GLE4, C5BAP9, A5F945, Q66EF1, B3E9X0, B0RP74, Q0T852, A4Y4G4, A1KG00, A6LSY8, A6Q9P9, Q8KAQ7, A8FFU9, B0U328, B9LZL6, A9N0P9, Q2G283, Q0SF42, Q15YL3, B3QRD2, C3K2K3, P71084, Q72K83, A9KSC7, Q32JV4, B8GJJ2, Q2FTK5, Q6GFJ3, A3PUB7, B1J1Y6, Q87LY3, C3L6Z2, B7UIK1, A8FLR2, A3DIF3, A7ZHP6, A7Z7A2, P0C2D9, Q9JRW9, B3QSA6, Q2A2U8, Q5PD43, A6UWB3, C0ZUX9, A2SQU3, O74061, A4IRG2, P0C1P8, P0CL07, A3MWW7, A4XC73, Q1LQM3, Q3AP59, Q3ACS9, A9GDD3, A5CNI7, Q8Y6J9, Q81I85, Q6HD65, A6TJD8, A6Q2X6, Q4FVC4, A4IKL1, B1JK22, Q0ST19, Q8FSD4, Q9PKI3, B9DZG0, Q976H2, A9VSS7, Q7VDA1, B2SGG7, B1HUT1, B1YK58, A1RQR5, Q4L706, A3N2K3, B4RNX2, Q07YU5, Q1QSB0, Q2S8X9, Q3JPN1, C1ETQ7, B8F7H5, B7GIK0, Q5FAH9, A9KP86, A5IC29, Q4L7G9, Q3AWP4, B1YUJ7, Q7WF71, A5EXX1, Q5P6J6, Q3A7W5, C4L4J9, A0R9G6, A6QHK1, B8HBR2, Q6FCY1, Q75G04, Q6G870, Q9K8G3, Q7V2J3, A7H3N1, Q6AHE8, Q1CUJ7, Q31FB1, B7N823, Q1DFA7, Q6AQ32, A6VUX8, P18492, P48247, A0KNY9, A7MGR5, A9WPI0, Q1GXW0, Q7MHY9, B7HU66, Q06741, B4SGW1, B0JPW6, P56115, Q0AAH7, C6AR33, A5W9H0, A5IU30, B7MBD7, P23893, Q4K5I6, B0UST3, Q2SYB2, B7H9S6, A5GUJ2, C1A7K7, A3NCF3, A1ST92, A8YY36, Q18ES5, A3MMQ8, Q5HUU3, A8G9U7, Q7P1Z5, Q8TYL6, B2TPD4, A8M6S5, A1SE06, B2J7M9, A1BJG8, B5Y1L5, Q8EHC8, A4SGT2, Q60CV0, B8CJG4, B3DY05, Q254Z2, Q6HNS8, B0VU92, Q725I1, B4EUE1, Q92AX5, A1V9X6, B4EBT3, C4LAK4, Q7V677, Q8X4V5, B0TIQ0, Q71ZB5, B9KFS8, Q5SJS4, B7IW22, Q88DP0, A5D3M2, B1MHH1, A2BL27, Q2JMP7, A0LIP3, B1LGV7, O26330, A1S3U0, Q46GT9, C3LSN1, Q63RP8, B2GL27, Q8NW75, Q49YQ9, B9LKS0, C1CWI8, B0SF64, B3PL68, A8M919, Q71YY2, Q14HS1, A1VSM6, A1ASE9, Q1MPW7, B2USD7, B1JX81, B2A1H4, A4T358, A6WKL6, P46716, A3CU65, P63508, O74038, Q40147, Q8EY44, B5BL82, Q8PH40, Q3ALU9, A5ITJ2, B4S0D0, Q73SQ3, A0LXY3, A4XK09, B0TFV0, Q92BG1, B9LA83, A1R898, B4TK30, Q12EF7, C0ZAH4, Q4JAM7, Q17X40, A1TYG5, Q2YU22, Q8ZYW1, A8ETJ2, O84212, B8HYK1, B2K547, Q6AB08, A2C0U2, Q24VD4, Q39566, Q83FJ5, Q9Y9I9, Q2JFQ1, A8H164, B1XD24, B1XIT5, B2U2Z9, B7V9D9, Q21YQ0, Q46CH1, P42799, Q30WH2, Q4ZNA0, Q0HG53, Q9HKM6, Q7N845, Q2NVQ0, B9IZ36, A0RXB3, Q0BHJ2, A4G8N0, B7NIB7, A7X3X9, Q3IHS1, C1AKK4, Q0W5T3, Q83AK3, Q06774, A4XYV6, B1Y8G2, C4KJ00, A0K5D7, A4FZY1, Q2FXR4, Q8CV56, A4TPW6, A5N5Y1, Q46XZ7, Q9ZMD0, Q3B1A1, Q48DP1, Q72ZW5, A2BPW6, B0SNK3, B5ERN9, Q6L2G9, Q81YV0, Q8DBX8, Q85WB7, B8G2L6, A9WIS7, B8ZT67, C0QCR9, A3NY82, Q7W050, Q3BPP7, B0B9W0, A4IXN8, B7MP16, Q5L2S4, P9WMN8, Q7VHK3, B3GYN8, A9NAX3, B1KHF6, Q4JSY1, A0PLS0, B3EKJ7, Q9F2S0, A1RMG7, B8J3A3, Q73DX4, A8LCD0, P45621, A8G3J9, A3QBN5, Q47LB3, A7HIX3, A7NCX8, Q97MU2, C1DMY5, A6V0D2, B2FT35, C4ZRP7, B7IHH3, B8DN02, B5Z0D4, A6URL2, A7MUU9, B9L0Q2, B9MRJ7, Q3IT20, Q2IHP8, P9WMN9, A1UAR1, C3PKI4, B7JQ54, B5EFG4, Q0BLC7, A5G9C0, B1YJU8, Q6NJJ2, Q817R3, A6W5M6, P30949, Q1CLU7, Q63GB4, Q821C1, B4S3Q6, B2SKS0, Q83H98, A6VQ66, B0CC57, Q8CRW7, E1W874, B1IQI6, Q0I3R7, Q3SFU6, Q478V1, B3EI07, Q13V40, Q2Y5Q5, B7VJJ5, Q47V96, B9J3N2, A5WC94, Q3M3B9, A7Z2N8, Q42522, B1X023, B1ZVF7, A1A7K0, B9DND8, A8ALD5, B8DHJ5, B7K2I1, Q1AUK6, C3LHA0, P24630, Q5HFA5, A4WN33, A8Z2I8, A2C7I7, A7GTE2, Q11WK1, B1YBL3, A1JJQ1, Q2S1S3, B7M195, A4VQY0, A4YD91, A5GMT2, B2HRL5, Q6G8Q8, Q04NV4, A3CL81, Q57T53, Q2NF42, Q2YTC2, Q8PW58, A7ZWA2, Q31C50, C0Q5R5, B7GH35, B7LWB5, B2HW19, C1DUY4, Q8D3C8, Q0AFV1, B2I6C2, Q6MAC7, P31593, Q2JS70, Q8CZE3, B9DMX3, Q8Z9B4, A4W6Q1, B9E740, C3MJ22, B5YHH6, A1TKK8, C3PCZ3, Q01YQ2, A0Q628, Q6LUS3, A2S9D9, A3M7I8, B1VEK3, Q6MHT9, Q3JDH7, Q9KEB0, B2T6C2, B8G822, C3NF69, B7IIX2, Q1I4H5, B4SUY4, A7FM09, Q65GK4, B7JNG6, Q2FG69, A9VIT5, Q5WEP8, A4QB78, Q1BYB1, A8ZZU9, A1AVQ1, A1V1L0, A0RQ51, B5R3G6, Q6M0P5, B2UNE3, B6HZD0, Q67KM3, A8FS76, C1EWG6, Q87VY5, Q7UPM9, Q12KC8, Q58020, A9R1E6, Q55665, Q5HNN6, B2JED5, Q8P5R4, B9LTZ9, A9M1G6, A2SKQ7, Q82E21, Q5ZVA6, A0B885, C3MZR9, Q897K4, Q5X529, Q1QEE8, A7I7P2, Q31QJ2, Q39IQ4, A7I252, C4L367, B4U8M6, A5TZQ4, B7HE93, Q2P6E4, B2U6Q7, B8I0R1, Q980U5, A9BY74, B7LGL6, Q0VSP6, C6DC32, Q8DLK8, B1HVD3, Q0TQG7, B7JBI1, A6GYW4, B4TXQ6, Q3Z5K3, Q9PP70, Q1IWZ8, A5VM65, A6T2A2, B9MF68, Q8FL16, Q0AZ36, B0BBJ0, A7ZCH5, B5FAL8, Q1BE73, B5F8R5, C1KVY4, Q5HER0, A1KS34, A8MGY8, B5RHE0, A6U2W8, A2BVE5, Q0RS03, B5FJ01, B7GYZ5, B8DFN7, A1WYL3, Q8TT57, B6EL04, B2V5U0, C0Z671, Q39QA6, Q0KDN9, Q0TLH7, A1VZJ6, B6J3H2, Q1RG34, B0VCN6, Q8CNZ1, Q9PB43, Q04X52, B1VTD1, Q2KUS4, B0BRF0, Q5H3I5, B8FBA1, Q9RWW0, Q5HN71, Q0I8G1, Q7NPI4, B1I4L1, Q1IHV2, Q74GA9, A6QI46, B7I4N4, A7GL00, B1XT79, Q7W3U1, B0U0T6, A0JYM2, Q633Y3, B4SI23, B0R7L9, A3D1R5, A0LRE5, Q6YZE2, Q7A4T5, Q49Y99, C1D9B6, O66998, Q1C3X1, A9A1A0, C1F911, A5FIM3, A1KB59, Q5L5P0, A1WMA0, A6VIL1, A1T3F2, A5CXH8, A0L3S9, Q5KWK9, A6U2D5, Q8YS26, A4SVE6, P63507, Q9JW10, A9BEA5, Q87BW3, B5ZA72, Q97B25, B2G9H2, Q110Z9, Q5YP79, Q9KU97, Q5WIE9, B7HQM1, B0KJV9, A7GXK4, Q6D1Z0, A9I1R3, Q12WM7, B3R312, Q5E2W6, A9A875, A0QR33, A9KBA0, A0QLG2, B6J495, Q5QVP9, A8AAB3, C1KVK0, Q5WWG1, Q99T15, A1WBR8, C3P9E6, Q8RFY7, A5UML0, Q5NGB9, Q5UZ90, Q0HSE6, Q4UYA7, Q8ZBL9, B7KA18, A7X388, Q8Y6X8, Q8NT73, Q21MJ0, Q2LVW6, B2UX41, B9E7Y3, Q325Y5, A8FB92, A5UU40, Q2RJ31, C1AZ30, Q3K6C0, Q62HV8, C4K6Y5, Q6GG38, A0Q2A8, Q822Q0, A7NKV1, Q7M847, A0AJD9, Q65M82, Q9JXW0, A4SJ79, Q30RJ4, O29027, Q9CNG9, Q82UQ8, Q65U43, Q8Y1M4, A3PBK8, C3MYE0, A9MPK7, A4J6H0, P99096, Q2FFN1, A4JC86, A6LKX4, Q9HMY8, A0RJ78, A9AEU0, C3N842, Q8NVU6, A4FPX3, B4UKE6, B6JKN5, C0QQ98, A9B550, Q7U598, A0KZS6, A6T4V8, Q3KMF2, A0AJ02, B8JCU6, B0RBL3, Q81LD0, Q02SE5, A9L5J5, B2VE25</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>pyruvate</t>
+          <t>oxaloacetate</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -913,78 +913,483 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>18.42954643596844</v>
+        <v>23.32996788924784</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.3014670514670515</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.1101010101010101</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.07207792207792207</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Q9KJF0</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Q643C8</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>G8FRC5</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>28.50228818719788</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.308047138047138</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1463636363636364</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Q5RAE3</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>O06644</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>26.37068917026454</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2663882413882414</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.7393162393162394</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.05984848484848485</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Q5P5Z3</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Q70AC7</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>24.35179810079771</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.308047138047138</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.1463636363636364</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Q5RAE3</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>O06644</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>25.15642465317967</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.4908831908831909</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.7393162393162394</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Q5P5Z3</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>P70712</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>30.05399799404772</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.308047138047138</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.1463636363636364</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Q5RAE3</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>O06644</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>31.91858953732631</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.4398148148148147</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>D5FKJ3</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>A7MBE0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>18.42954643860628</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.2804713804713804</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.06363636363636363</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Q5RAE3</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Q70AC7</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>32.96197984318157</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.2464387464387464</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.7393162393162394</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Q5P5Z3</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>P39976</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>28.0388590838786</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.4106125356125356</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.4540598290598291</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Q70AC7</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>A9WGE3, Q1KLK0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>pyruvate</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>8.492261080996217</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.2265151515151515</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.5833333333333334</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.09621212121212121</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Q88JX9, A5W059</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>B8EBU3, B8GLE4, C5BAP9, A5F945, Q66EF1, B3E9X0, B0RP74, Q0T852, A4Y4G4, A1KG00, A6LSY8, A6Q9P9, Q8KAQ7, A8FFU9, B0U328, B9LZL6, A9N0P9, Q2G283, Q0SF42, Q15YL3, B3QRD2, C3K2K3, P71084, Q72K83, A9KSC7, Q32JV4, B8GJJ2, Q2FTK5, Q6GFJ3, A3PUB7, B1J1Y6, Q87LY3, C3L6Z2, B7UIK1, A8FLR2, A3DIF3, A7ZHP6, A7Z7A2, P0C2D9, Q9JRW9, B3QSA6, Q2A2U8, Q5PD43, A6UWB3, C0ZUX9, A2SQU3, O74061, A4IRG2, P0C1P8, P0CL07, A3MWW7, A4XC73, Q1LQM3, Q3AP59, Q3ACS9, A9GDD3, A5CNI7, Q8Y6J9, Q81I85, Q6HD65, A6TJD8, A6Q2X6, Q4FVC4, A4IKL1, B1JK22, Q0ST19, Q8FSD4, Q9PKI3, B9DZG0, Q976H2, A9VSS7, Q7VDA1, B2SGG7, B1HUT1, B1YK58, A1RQR5, Q4L706, A3N2K3, B4RNX2, Q07YU5, Q1QSB0, Q2S8X9, Q3JPN1, C1ETQ7, B8F7H5, B7GIK0, Q5FAH9, A9KP86, A5IC29, Q4L7G9, Q3AWP4, B1YUJ7, Q7WF71, A5EXX1, Q5P6J6, Q3A7W5, C4L4J9, A0R9G6, A6QHK1, B8HBR2, Q6FCY1, Q75G04, Q6G870, Q9K8G3, Q7V2J3, A7H3N1, Q6AHE8, Q1CUJ7, Q31FB1, B7N823, Q1DFA7, Q6AQ32, A6VUX8, P18492, P48247, A0KNY9, A7MGR5, A9WPI0, Q1GXW0, Q7MHY9, B7HU66, Q06741, B4SGW1, B0JPW6, P56115, Q0AAH7, C6AR33, A5W9H0, A5IU30, B7MBD7, P23893, Q4K5I6, B0UST3, Q2SYB2, B7H9S6, A5GUJ2, C1A7K7, A3NCF3, A1ST92, A8YY36, Q18ES5, A3MMQ8, Q5HUU3, A8G9U7, Q7P1Z5, Q8TYL6, B2TPD4, A8M6S5, A1SE06, B2J7M9, A1BJG8, B5Y1L5, Q8EHC8, A4SGT2, Q60CV0, B8CJG4, B3DY05, Q254Z2, Q6HNS8, B0VU92, Q725I1, B4EUE1, Q92AX5, A1V9X6, B4EBT3, C4LAK4, Q7V677, Q8X4V5, B0TIQ0, Q71ZB5, B9KFS8, Q5SJS4, B7IW22, Q88DP0, A5D3M2, B1MHH1, A2BL27, Q2JMP7, A0LIP3, B1LGV7, O26330, A1S3U0, Q46GT9, C3LSN1, Q63RP8, B2GL27, Q8NW75, Q49YQ9, B9LKS0, C1CWI8, B0SF64, B3PL68, A8M919, Q71YY2, Q14HS1, A1VSM6, A1ASE9, Q1MPW7, B2USD7, B1JX81, B2A1H4, A4T358, A6WKL6, P46716, A3CU65, P63508, O74038, Q40147, Q8EY44, B5BL82, Q8PH40, Q3ALU9, A5ITJ2, B4S0D0, Q73SQ3, A0LXY3, A4XK09, B0TFV0, Q92BG1, B9LA83, A1R898, B4TK30, Q12EF7, C0ZAH4, Q4JAM7, Q17X40, A1TYG5, Q2YU22, Q8ZYW1, A8ETJ2, O84212, B8HYK1, B2K547, Q6AB08, A2C0U2, Q24VD4, Q39566, Q83FJ5, Q9Y9I9, Q2JFQ1, A8H164, B1XD24, B1XIT5, B2U2Z9, B7V9D9, Q21YQ0, Q46CH1, P42799, Q30WH2, Q4ZNA0, Q0HG53, Q9HKM6, Q7N845, Q2NVQ0, B9IZ36, A0RXB3, Q0BHJ2, A4G8N0, B7NIB7, A7X3X9, Q3IHS1, C1AKK4, Q0W5T3, Q83AK3, Q06774, A4XYV6, B1Y8G2, C4KJ00, A0K5D7, A4FZY1, Q2FXR4, Q8CV56, A4TPW6, A5N5Y1, Q46XZ7, Q9ZMD0, Q3B1A1, Q48DP1, Q72ZW5, A2BPW6, B0SNK3, B5ERN9, Q6L2G9, Q81YV0, Q8DBX8, Q85WB7, B8G2L6, A9WIS7, B8ZT67, C0QCR9, A3NY82, Q7W050, Q3BPP7, B0B9W0, A4IXN8, B7MP16, Q5L2S4, P9WMN8, Q7VHK3, B3GYN8, A9NAX3, B1KHF6, Q4JSY1, A0PLS0, B3EKJ7, Q9F2S0, A1RMG7, B8J3A3, Q73DX4, A8LCD0, P45621, A8G3J9, A3QBN5, Q47LB3, A7HIX3, A7NCX8, Q97MU2, C1DMY5, A6V0D2, B2FT35, C4ZRP7, B7IHH3, B8DN02, B5Z0D4, A6URL2, A7MUU9, B9L0Q2, B9MRJ7, Q3IT20, Q2IHP8, P9WMN9, A1UAR1, C3PKI4, B7JQ54, B5EFG4, Q0BLC7, A5G9C0, B1YJU8, Q6NJJ2, Q817R3, A6W5M6, P30949, Q1CLU7, Q63GB4, Q821C1, B4S3Q6, B2SKS0, Q83H98, A6VQ66, B0CC57, Q8CRW7, E1W874, B1IQI6, Q0I3R7, Q3SFU6, Q478V1, B3EI07, Q13V40, Q2Y5Q5, B7VJJ5, Q47V96, B9J3N2, A5WC94, Q3M3B9, A7Z2N8, Q42522, B1X023, B1ZVF7, A1A7K0, B9DND8, A8ALD5, B8DHJ5, B7K2I1, Q1AUK6, C3LHA0, P24630, Q5HFA5, A4WN33, A8Z2I8, A2C7I7, A7GTE2, Q11WK1, B1YBL3, A1JJQ1, Q2S1S3, B7M195, A4VQY0, A4YD91, A5GMT2, B2HRL5, Q6G8Q8, Q04NV4, A3CL81, Q57T53, Q2NF42, Q2YTC2, Q8PW58, A7ZWA2, Q31C50, C0Q5R5, B7GH35, B7LWB5, B2HW19, C1DUY4, Q8D3C8, Q0AFV1, B2I6C2, Q6MAC7, P31593, Q2JS70, Q8CZE3, B9DMX3, Q8Z9B4, A4W6Q1, B9E740, C3MJ22, B5YHH6, A1TKK8, C3PCZ3, Q01YQ2, A0Q628, Q6LUS3, A2S9D9, A3M7I8, B1VEK3, Q6MHT9, Q3JDH7, Q9KEB0, B2T6C2, B8G822, C3NF69, B7IIX2, Q1I4H5, B4SUY4, A7FM09, Q65GK4, B7JNG6, Q2FG69, A9VIT5, Q5WEP8, A4QB78, Q1BYB1, A8ZZU9, A1AVQ1, A1V1L0, A0RQ51, B5R3G6, Q6M0P5, B2UNE3, B6HZD0, Q67KM3, A8FS76, C1EWG6, Q87VY5, Q7UPM9, Q12KC8, Q58020, A9R1E6, Q55665, Q5HNN6, B2JED5, Q8P5R4, B9LTZ9, A9M1G6, A2SKQ7, Q82E21, Q5ZVA6, A0B885, C3MZR9, Q897K4, Q5X529, Q1QEE8, A7I7P2, Q31QJ2, Q39IQ4, A7I252, C4L367, B4U8M6, A5TZQ4, B7HE93, Q2P6E4, B2U6Q7, B8I0R1, Q980U5, A9BY74, B7LGL6, Q0VSP6, C6DC32, Q8DLK8, B1HVD3, Q0TQG7, B7JBI1, A6GYW4, B4TXQ6, Q3Z5K3, Q9PP70, Q1IWZ8, A5VM65, A6T2A2, B9MF68, Q8FL16, Q0AZ36, B0BBJ0, A7ZCH5, B5FAL8, Q1BE73, B5F8R5, C1KVY4, Q5HER0, A1KS34, A8MGY8, B5RHE0, A6U2W8, A2BVE5, Q0RS03, B5FJ01, B7GYZ5, B8DFN7, A1WYL3, Q8TT57, B6EL04, B2V5U0, C0Z671, Q39QA6, Q0KDN9, Q0TLH7, A1VZJ6, B6J3H2, Q1RG34, B0VCN6, Q8CNZ1, Q9PB43, Q04X52, B1VTD1, Q2KUS4, B0BRF0, Q5H3I5, B8FBA1, Q9RWW0, Q5HN71, Q0I8G1, Q7NPI4, B1I4L1, Q1IHV2, Q74GA9, A6QI46, B7I4N4, A7GL00, B1XT79, Q7W3U1, B0U0T6, A0JYM2, Q633Y3, B4SI23, B0R7L9, A3D1R5, A0LRE5, Q6YZE2, Q7A4T5, Q49Y99, C1D9B6, O66998, Q1C3X1, A9A1A0, C1F911, A5FIM3, A1KB59, Q5L5P0, A1WMA0, A6VIL1, A1T3F2, A5CXH8, A0L3S9, Q5KWK9, A6U2D5, Q8YS26, A4SVE6, P63507, Q9JW10, A9BEA5, Q87BW3, B5ZA72, Q97B25, B2G9H2, Q110Z9, Q5YP79, Q9KU97, Q5WIE9, B7HQM1, B0KJV9, A7GXK4, Q6D1Z0, A9I1R3, Q12WM7, B3R312, Q5E2W6, A9A875, A0QR33, A9KBA0, A0QLG2, B6J495, Q5QVP9, A8AAB3, C1KVK0, Q5WWG1, Q99T15, A1WBR8, C3P9E6, Q8RFY7, A5UML0, Q5NGB9, Q5UZ90, Q0HSE6, Q4UYA7, Q8ZBL9, B7KA18, A7X388, Q8Y6X8, Q8NT73, Q21MJ0, Q2LVW6, B2UX41, B9E7Y3, Q325Y5, A8FB92, A5UU40, Q2RJ31, C1AZ30, Q3K6C0, Q62HV8, C4K6Y5, Q6GG38, A0Q2A8, Q822Q0, A7NKV1, Q7M847, A0AJD9, Q65M82, Q9JXW0, A4SJ79, Q30RJ4, O29027, Q9CNG9, Q82UQ8, Q65U43, Q8Y1M4, A3PBK8, C3MYE0, A9MPK7, A4J6H0, P99096, Q2FFN1, A4JC86, A6LKX4, Q9HMY8, A0RJ78, A9AEU0, C3N842, Q8NVU6, A4FPX3, B4UKE6, B6JKN5, C0QQ98, A9B550, Q7U598, A0KZS6, A6T4V8, Q3KMF2, A0AJ02, B8JCU6, B0RBL3, Q81LD0, Q02SE5, A9L5J5, B2VE25</t>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>oxaloacetate</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>21.85918311167207</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.3053276353276353</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.7393162393162394</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1766666666666667</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Q5P5Z3</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>O06644</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1471,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1082,36 +1487,36 @@
         <v>3.287398429598943</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7037037037037037</v>
+        <v>0.6972934472934473</v>
       </c>
       <c r="F2" t="n">
-        <v>0.75</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.7307692307692308</v>
       </c>
       <c r="H2" t="n">
         <v>0.5833333333333334</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Q01772</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>H8ZPX2</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>P26263, P16467</t>
+          <t>P06169</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1127,10 +1532,10 @@
         <v>3.287398429602959</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7870370370370371</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.8472222222222222</v>
       </c>
       <c r="G3" t="n">
         <v>0.7777777777777777</v>
@@ -1140,7 +1545,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>A0QMB9, P38067, P94428, P9WNX6, A0R4Q0, Q7TZP3, P9WNX9, A0PST9, P25526, P9WNX7, A0PN13, O32507, Q55585, A1KJE8, Q73TP5, O69497, A5TYV9, P9WNX8, A1KF54, P55653, A5U390</t>
+          <t>A0QTU8</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1150,7 +1555,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>P26263, P16467</t>
+          <t>P06169</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1232,7 +1637,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1248,36 +1653,36 @@
         <v>20.97839160986774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2542087542087542</v>
+        <v>0.2361111111111111</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7626262626262625</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>G9M9M4</t>
+          <t>F1R4U0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>Q58991</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Q1KLK1, Q1KLK0, A9WC40</t>
+          <t>Q588Z2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1290,39 +1695,39 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20.97826328754108</v>
+        <v>27.49964885187668</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04545454545454545</v>
+        <v>0.4927048260381593</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.6851851851851851</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.7929292929292929</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1363636363636364</v>
+        <v>0</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>P39976</t>
+          <t>P76621</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>B7GQR3, O67480, P56574, Q40345, Q6C2Y4, P50218, O53611, Q75JR2, Q9ZN36, A5U813, P20304, Q8RQL9, Q06197, A8YGS2, P65099, P83726, Q9X0N2, Q9SRZ6, P41939, Q4E4L7, Q9YE81, Q9Z2K9, B2ZP83, Q4UKR1, P50217, Q68XA5, P65098, B2ZAA4, P99167, Q6XUZ5, O29610, Q8NW61, Q8U488, P50214, Q5R9C5, O88844, Q9Z2K8, Q5HF79, Q8L0X8, P21954, P96318, P50216, Q59940, Q9ZDR0, P50215, Q9CHQ4, Q8LPJ5, D7RIE8, Q1XIQ8, Q9XSG3, O75874, P9WKL0, Q4DG65, P41561, P56063, P80046, P9WKL1, Q6AQ66, Q6GG12, Q9HLV8, Q02NB5, Q6G8N2, P08200, O14254, Q92IR7, O13294, P48735, P16100, P41560, Q59985, J9Q6L4, P79089, P41562, Q1XIQ9, Q8CNX4, Q4R502, P33198, Q75JR3, O65853, P39126, O13285, D4GU92, Q9ZH99, Q5HNL1, Q6R6M7, Q9SLK0, Q04467, P53982, B4FLJ3, P54071, P33197, Q1RJU4</t>
+          <t>Q46N53</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>P0C017, O28997, P21264, P55195, P50504, Q01930, P15567, P22234, P0CQ36, Q73PV9, Q9UVE6, O74197, O80937, P0CQ37, Q92210</t>
+          <t>P31572</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1335,23 +1740,23 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>27.49964885187668</v>
+        <v>27.49964883551251</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4741863075196409</v>
+        <v>0.2542087542087542</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6296296296296297</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7929292929292929</v>
+        <v>0.7626262626262625</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Q92LF6, Q989T9</t>
+          <t>Q1GNW5</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1361,7 +1766,52 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Q1KLK1, Q1KLK0, A9WC40</t>
+          <t>A9WGE3, Q1KLK0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>malate</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>20.97826328754108</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2542087542087542</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.7626262626262625</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>P76621</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Q46N53</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>A9WGE3, Q1KLK0</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1443,11 +1893,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1456,43 +1906,43 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>28.0388590838786</v>
+        <v>15.85866290964453</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6791310541310541</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4540598290598291</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8055555555555555</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>A5W059</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>E3PY95</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>E9RFT1, E9RFS9</t>
+          <t>Q588Z2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1501,43 +1951,43 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>18.42954643860628</v>
+        <v>58.23487147501859</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5731481481481481</v>
+        <v>0.5799663299663299</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.1287878787878788</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>D5FKJ3</t>
+          <t>E3PY95</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Q59268</t>
+          <t>Q9QYF1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1546,43 +1996,43 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>25.71247087886662</v>
+        <v>18.42954643354551</v>
       </c>
       <c r="E4" t="n">
-        <v>0.568097643097643</v>
+        <v>0.5257335257335257</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.1287878787878788</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7626262626262625</v>
+        <v>0.6428571428571428</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4</v>
+        <v>0.8055555555555555</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Q643C8</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Q5PDP3, Q989E7, Q3A133, Q9A5V1, P62456, Q02136, Q57MS3, Q606Q2, Q8XV79, Q46WL2, Q2P3K3, Q5LL27, Q82AA6, Q8EFB1, Q5WDH8, Q8ESR8, P16245, P62458, Q8YSM8, Q313T7, Q8YWL4, Q5QWP8, Q3Z878, P60862, Q4JW59, Q2RGV8, Q39K91, Q8P9P2, Q5ZW87, A0A0J9X7D2, Q97KI2, Q9K6Z2, P06988, Q47XB8, Q8PLG9, Q3MEV7, Q6D411, O34651, Q5V574, A1BPP9, Q722Y3, P60859, Q9PBC5, Q30TA4, Q8TXG3, P24226, Q7V5N9, Q92S26, Q9RQ88, Q5F7D8, Q8ZFX5, Q7VFF5, Q5HKN8, Q47AL5, P62457, Q39YP7, Q9JTH9, Q8ZY17, Q7NL02, O33775, Q6FEC8, Q323J2, Q5FS83, Q8R882, Q8F393, P62460, Q7M8K9, Q9HPW5, B0SS41, B0S9F2, Q65EF9, Q62GD9, Q5SKC1, Q3J7H1, Q4A044, Q63DX2, Q2YAU5, Q8D8Q0, Q318Q4, Q46J19, Q8G2R2, Q3AD53, Q6G5Z7, Q7WDY4, Q9P777, Q5E638, Q4FNE2, Q845V3, Q7VQX0, Q5KVC6, Q8G4S9, Q4QN74, Q8GKZ1, Q9ZHE6, Q3ICF0, Q3Z0G5, Q3J079, Q58851, O59626, Q48EC9, P44001, P63954, Q7W2Y4, P73058, Q9RSI4, Q87QL1, Q8X8T3, O26327, Q3ZXL7, Q81G06, Q8GDP4, P60861, Q4ZNV9, Q7V004, Q6HLE7, Q9RQ85, P18786, Q8DGR2, Q3B5E3, Q65RB1, P63953, Q8Z5K0, Q5X5W9, Q82W26, Q8UHX1, P9WNW8, Q5WX91, P60858, Q7VA26, Q8Y9G1, Q5HCL9, Q6GDC6, Q9CLM4, Q8ABA9, Q9C5U8, P59397, Q4J8I8, P10370, Q3SW26, Q5YYQ0, Q6A8L5, Q5MZ26, Q6AE76, Q8FG52, Q7U8K7, Q9L6I1, P63951, Q3JMZ6, Q7MLS6, Q9JYH8, Q8FNZ0, Q47QS9, Q3BUF7, Q4UU40, Q9RH05, Q3M5D3, Q7P0F6, Q8NNT5, Q31GY9, Q8DTQ7, Q492K3, Q2YZB4, Q57F99, Q81T62, P28736, Q2YPB8, Q5LAZ8, P9WNW9, P59398, P59400, O66976, P60860, P63952, O30027, Q5HSJ3, Q2RQM7, Q9HVW9, P62459, Q8PZR8, P59399, Q87C29, Q9F854, Q87WV5, Q9CC57, Q5P790, Q3AR25, Q8YF59, Q465R4, P59401, Q9X0D1, Q7VSZ1, Q7UX39, Q3SI67, Q63Q86, Q66C49, Q92E84, P57201, Q5H0L1, Q5JFR5, Q8CQ95, Q5NAY4, Q9PM77, Q970Y9, Q4FQF8, Q8TL41, Q6ANR3, Q3KHZ2, Q64RE7, Q6KZD1, Q9RQ82, Q8KEY6, Q67KH6, Q4KI73, Q32EE9</t>
+          <t>Q9S5G5</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Q59268</t>
+          <t>A0QTU8</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1591,43 +2041,43 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>26.56969255872742</v>
+        <v>11.89198569423518</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3282652532652533</v>
+        <v>0.3285353535353536</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1101010101010101</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1524725274725275</v>
+        <v>0.06893939393939394</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>A5W059</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>E3PY95</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1636,43 +2086,43 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>29.73474970552454</v>
+        <v>18.42954643596844</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5274410774410775</v>
+        <v>0.2572150072150072</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1101010101010101</v>
+        <v>0.1287878787878788</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.6428571428571428</v>
       </c>
       <c r="H6" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>Q9S5G5</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Q588Z2</t>
+          <t>P31572</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1681,43 +2131,43 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>28.50228818719788</v>
+        <v>32.04739186446719</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5361531986531985</v>
+        <v>0.2236842105263158</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G7" t="n">
-        <v>0.08068181818181819</v>
+        <v>0.08771929824561403</v>
       </c>
       <c r="H7" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>A5W059</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>B6E2X2</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Q588Z2</t>
+          <t>A7MBE0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1726,43 +2176,43 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>24.35179810079771</v>
+        <v>45.54604734856605</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3101791726791727</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="G8" t="n">
-        <v>0.08068181818181819</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.07207792207792207</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>D5FKJ3</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>G8FRC5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1771,43 +2221,43 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>25.15642465317967</v>
+        <v>8.492261080996217</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3014670514670515</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1101010101010101</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="H9" t="n">
-        <v>0.07207792207792207</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>P39976</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>D5FKJ3</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>G8FRC5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1816,43 +2266,43 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>24.24741408404559</v>
+        <v>11.89198569708731</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3101791726791727</v>
+        <v>0.2265151515151515</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G10" t="n">
-        <v>0.08068181818181819</v>
+        <v>0.09621212121212121</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07207792207792207</v>
+        <v>0</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>A5W059</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>A7MBE0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1861,43 +2311,43 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>32.96197984318157</v>
+        <v>7.90381435109191</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3014670514670515</v>
+        <v>0.3392255892255893</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1101010101010101</v>
+        <v>0.1287878787878788</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H11" t="n">
-        <v>0.07207792207792207</v>
+        <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>F4I907</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
+          <t>A7MBE0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>oxaloacetate</t>
+          <t>pyruvate</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1906,438 +2356,33 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>21.85918311167207</v>
+        <v>8.492132758669902</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3053276353276353</v>
+        <v>0.2361111111111111</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.7393162393162394</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1766666666666667</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Q9KJF0</t>
+          <t>P39976</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Q46N53</t>
+          <t>Q70AC7</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Q89QH2, A4YXN2, B3QBS6, Q8XBR7, B7M6P3, A4G242, A5EGD7, Q46S66, Q2IUI7, B1X9P6, Q31Y97, Q6N8F8, B1IX88, A7ZPI2, B1LMH0, Q217M3, Q46S72, A4G241, Q8FFE8, B6JE29, B7NPQ8, C4ZVR1, A7ICK2, B7UG84, Q0TF87, Q82M40, A6T0J2, B2TWX3, Q0K0H8, A9X6P7, O87838, Q3YZF6, B5YYX4, P69902, Q07Q82, Q1R8Z2, B6I6S5, A8A2M8, Q13RQ4, B7LBS7, P69903, O06644, B7MH34, Q32DG9, B7MY33, A1ADQ1, B7N5X4, Q139H7</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>24.36708975704198</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.2464387464387464</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.7393162393162394</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Q8BGT5, O07597, Q6GM82, Q8NW24, P52893, P34106, X5DUP7, P54692, P0A961, P52894, Q5HF24, Q9LDV4, Q71Z49, P71348, G2JZ74, P54694, Q8QZR5, P13191, P99090, Q5HNG0, P19938, Q6NYL5, P0A960, P0A959, P54693, Q10334, A4IFH5, Q8CS41, P25409, P63511, P24298, Q6G8H7, Q92B90, Q28DB5, P77434, Q54MJ7, F4I7I0, P52892, Q8TD30, X5DCE6, Q6GFV1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>31.91858953732631</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.4106125356125356</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.4540598290598291</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Q1KLK1, Q1KLK0, A9WC40</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>27.3588077454217</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.4106125356125356</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.4540598290598291</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Q1KLK1, Q1KLK0, A9WC40</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>24.35179694036886</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.2804713804713804</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.06363636363636363</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>30.05399799404772</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.2663882413882414</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.7393162393162394</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.05984848484848485</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>P02904, Q70AC7, Q8GBW6</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>21.91006321265886</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.308047138047138</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.1463636363636364</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Q89QH2, A4YXN2, B3QBS6, Q8XBR7, B7M6P3, A4G242, A5EGD7, Q46S66, Q2IUI7, B1X9P6, Q31Y97, Q6N8F8, B1IX88, A7ZPI2, B1LMH0, Q217M3, Q46S72, A4G241, Q8FFE8, B6JE29, B7NPQ8, C4ZVR1, A7ICK2, B7UG84, Q0TF87, Q82M40, A6T0J2, B2TWX3, Q0K0H8, A9X6P7, O87838, Q3YZF6, B5YYX4, P69902, Q07Q82, Q1R8Z2, B6I6S5, A8A2M8, Q13RQ4, B7LBS7, P69903, O06644, B7MH34, Q32DG9, B7MY33, A1ADQ1, B7N5X4, Q139H7</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>23.1305084350496</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.308047138047138</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.1463636363636364</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Q89QH2, A4YXN2, B3QBS6, Q8XBR7, B7M6P3, A4G242, A5EGD7, Q46S66, Q2IUI7, B1X9P6, Q31Y97, Q6N8F8, B1IX88, A7ZPI2, B1LMH0, Q217M3, Q46S72, A4G241, Q8FFE8, B6JE29, B7NPQ8, C4ZVR1, A7ICK2, B7UG84, Q0TF87, Q82M40, A6T0J2, B2TWX3, Q0K0H8, A9X6P7, O87838, Q3YZF6, B5YYX4, P69902, Q07Q82, Q1R8Z2, B6I6S5, A8A2M8, Q13RQ4, B7LBS7, P69903, O06644, B7MH34, Q32DG9, B7MY33, A1ADQ1, B7N5X4, Q139H7</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>26.37068917026454</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.4398148148148147</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.5416666666666666</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>D5FKJ3</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>B8EBU3, B8GLE4, C5BAP9, A5F945, Q66EF1, B3E9X0, B0RP74, Q0T852, A4Y4G4, A1KG00, A6LSY8, A6Q9P9, Q8KAQ7, A8FFU9, B0U328, B9LZL6, A9N0P9, Q2G283, Q0SF42, Q15YL3, B3QRD2, C3K2K3, P71084, Q72K83, A9KSC7, Q32JV4, B8GJJ2, Q2FTK5, Q6GFJ3, A3PUB7, B1J1Y6, Q87LY3, C3L6Z2, B7UIK1, A8FLR2, A3DIF3, A7ZHP6, A7Z7A2, P0C2D9, Q9JRW9, B3QSA6, Q2A2U8, Q5PD43, A6UWB3, C0ZUX9, A2SQU3, O74061, A4IRG2, P0C1P8, P0CL07, A3MWW7, A4XC73, Q1LQM3, Q3AP59, Q3ACS9, A9GDD3, A5CNI7, Q8Y6J9, Q81I85, Q6HD65, A6TJD8, A6Q2X6, Q4FVC4, A4IKL1, B1JK22, Q0ST19, Q8FSD4, Q9PKI3, B9DZG0, Q976H2, A9VSS7, Q7VDA1, B2SGG7, B1HUT1, B1YK58, A1RQR5, Q4L706, A3N2K3, B4RNX2, Q07YU5, Q1QSB0, Q2S8X9, Q3JPN1, C1ETQ7, B8F7H5, B7GIK0, Q5FAH9, A9KP86, A5IC29, Q4L7G9, Q3AWP4, B1YUJ7, Q7WF71, A5EXX1, Q5P6J6, Q3A7W5, C4L4J9, A0R9G6, A6QHK1, B8HBR2, Q6FCY1, Q75G04, Q6G870, Q9K8G3, Q7V2J3, A7H3N1, Q6AHE8, Q1CUJ7, Q31FB1, B7N823, Q1DFA7, Q6AQ32, A6VUX8, P18492, P48247, A0KNY9, A7MGR5, A9WPI0, Q1GXW0, Q7MHY9, B7HU66, Q06741, B4SGW1, B0JPW6, P56115, Q0AAH7, C6AR33, A5W9H0, A5IU30, B7MBD7, P23893, Q4K5I6, B0UST3, Q2SYB2, B7H9S6, A5GUJ2, C1A7K7, A3NCF3, A1ST92, A8YY36, Q18ES5, A3MMQ8, Q5HUU3, A8G9U7, Q7P1Z5, Q8TYL6, B2TPD4, A8M6S5, A1SE06, B2J7M9, A1BJG8, B5Y1L5, Q8EHC8, A4SGT2, Q60CV0, B8CJG4, B3DY05, Q254Z2, Q6HNS8, B0VU92, Q725I1, B4EUE1, Q92AX5, A1V9X6, B4EBT3, C4LAK4, Q7V677, Q8X4V5, B0TIQ0, Q71ZB5, B9KFS8, Q5SJS4, B7IW22, Q88DP0, A5D3M2, B1MHH1, A2BL27, Q2JMP7, A0LIP3, B1LGV7, O26330, A1S3U0, Q46GT9, C3LSN1, Q63RP8, B2GL27, Q8NW75, Q49YQ9, B9LKS0, C1CWI8, B0SF64, B3PL68, A8M919, Q71YY2, Q14HS1, A1VSM6, A1ASE9, Q1MPW7, B2USD7, B1JX81, B2A1H4, A4T358, A6WKL6, P46716, A3CU65, P63508, O74038, Q40147, Q8EY44, B5BL82, Q8PH40, Q3ALU9, A5ITJ2, B4S0D0, Q73SQ3, A0LXY3, A4XK09, B0TFV0, Q92BG1, B9LA83, A1R898, B4TK30, Q12EF7, C0ZAH4, Q4JAM7, Q17X40, A1TYG5, Q2YU22, Q8ZYW1, A8ETJ2, O84212, B8HYK1, B2K547, Q6AB08, A2C0U2, Q24VD4, Q39566, Q83FJ5, Q9Y9I9, Q2JFQ1, A8H164, B1XD24, B1XIT5, B2U2Z9, B7V9D9, Q21YQ0, Q46CH1, P42799, Q30WH2, Q4ZNA0, Q0HG53, Q9HKM6, Q7N845, Q2NVQ0, B9IZ36, A0RXB3, Q0BHJ2, A4G8N0, B7NIB7, A7X3X9, Q3IHS1, C1AKK4, Q0W5T3, Q83AK3, Q06774, A4XYV6, B1Y8G2, C4KJ00, A0K5D7, A4FZY1, Q2FXR4, Q8CV56, A4TPW6, A5N5Y1, Q46XZ7, Q9ZMD0, Q3B1A1, Q48DP1, Q72ZW5, A2BPW6, B0SNK3, B5ERN9, Q6L2G9, Q81YV0, Q8DBX8, Q85WB7, B8G2L6, A9WIS7, B8ZT67, C0QCR9, A3NY82, Q7W050, Q3BPP7, B0B9W0, A4IXN8, B7MP16, Q5L2S4, P9WMN8, Q7VHK3, B3GYN8, A9NAX3, B1KHF6, Q4JSY1, A0PLS0, B3EKJ7, Q9F2S0, A1RMG7, B8J3A3, Q73DX4, A8LCD0, P45621, A8G3J9, A3QBN5, Q47LB3, A7HIX3, A7NCX8, Q97MU2, C1DMY5, A6V0D2, B2FT35, C4ZRP7, B7IHH3, B8DN02, B5Z0D4, A6URL2, A7MUU9, B9L0Q2, B9MRJ7, Q3IT20, Q2IHP8, P9WMN9, A1UAR1, C3PKI4, B7JQ54, B5EFG4, Q0BLC7, A5G9C0, B1YJU8, Q6NJJ2, Q817R3, A6W5M6, P30949, Q1CLU7, Q63GB4, Q821C1, B4S3Q6, B2SKS0, Q83H98, A6VQ66, B0CC57, Q8CRW7, E1W874, B1IQI6, Q0I3R7, Q3SFU6, Q478V1, B3EI07, Q13V40, Q2Y5Q5, B7VJJ5, Q47V96, B9J3N2, A5WC94, Q3M3B9, A7Z2N8, Q42522, B1X023, B1ZVF7, A1A7K0, B9DND8, A8ALD5, B8DHJ5, B7K2I1, Q1AUK6, C3LHA0, P24630, Q5HFA5, A4WN33, A8Z2I8, A2C7I7, A7GTE2, Q11WK1, B1YBL3, A1JJQ1, Q2S1S3, B7M195, A4VQY0, A4YD91, A5GMT2, B2HRL5, Q6G8Q8, Q04NV4, A3CL81, Q57T53, Q2NF42, Q2YTC2, Q8PW58, A7ZWA2, Q31C50, C0Q5R5, B7GH35, B7LWB5, B2HW19, C1DUY4, Q8D3C8, Q0AFV1, B2I6C2, Q6MAC7, P31593, Q2JS70, Q8CZE3, B9DMX3, Q8Z9B4, A4W6Q1, B9E740, C3MJ22, B5YHH6, A1TKK8, C3PCZ3, Q01YQ2, A0Q628, Q6LUS3, A2S9D9, A3M7I8, B1VEK3, Q6MHT9, Q3JDH7, Q9KEB0, B2T6C2, B8G822, C3NF69, B7IIX2, Q1I4H5, B4SUY4, A7FM09, Q65GK4, B7JNG6, Q2FG69, A9VIT5, Q5WEP8, A4QB78, Q1BYB1, A8ZZU9, A1AVQ1, A1V1L0, A0RQ51, B5R3G6, Q6M0P5, B2UNE3, B6HZD0, Q67KM3, A8FS76, C1EWG6, Q87VY5, Q7UPM9, Q12KC8, Q58020, A9R1E6, Q55665, Q5HNN6, B2JED5, Q8P5R4, B9LTZ9, A9M1G6, A2SKQ7, Q82E21, Q5ZVA6, A0B885, C3MZR9, Q897K4, Q5X529, Q1QEE8, A7I7P2, Q31QJ2, Q39IQ4, A7I252, C4L367, B4U8M6, A5TZQ4, B7HE93, Q2P6E4, B2U6Q7, B8I0R1, Q980U5, A9BY74, B7LGL6, Q0VSP6, C6DC32, Q8DLK8, B1HVD3, Q0TQG7, B7JBI1, A6GYW4, B4TXQ6, Q3Z5K3, Q9PP70, Q1IWZ8, A5VM65, A6T2A2, B9MF68, Q8FL16, Q0AZ36, B0BBJ0, A7ZCH5, B5FAL8, Q1BE73, B5F8R5, C1KVY4, Q5HER0, A1KS34, A8MGY8, B5RHE0, A6U2W8, A2BVE5, Q0RS03, B5FJ01, B7GYZ5, B8DFN7, A1WYL3, Q8TT57, B6EL04, B2V5U0, C0Z671, Q39QA6, Q0KDN9, Q0TLH7, A1VZJ6, B6J3H2, Q1RG34, B0VCN6, Q8CNZ1, Q9PB43, Q04X52, B1VTD1, Q2KUS4, B0BRF0, Q5H3I5, B8FBA1, Q9RWW0, Q5HN71, Q0I8G1, Q7NPI4, B1I4L1, Q1IHV2, Q74GA9, A6QI46, B7I4N4, A7GL00, B1XT79, Q7W3U1, B0U0T6, A0JYM2, Q633Y3, B4SI23, B0R7L9, A3D1R5, A0LRE5, Q6YZE2, Q7A4T5, Q49Y99, C1D9B6, O66998, Q1C3X1, A9A1A0, C1F911, A5FIM3, A1KB59, Q5L5P0, A1WMA0, A6VIL1, A1T3F2, A5CXH8, A0L3S9, Q5KWK9, A6U2D5, Q8YS26, A4SVE6, P63507, Q9JW10, A9BEA5, Q87BW3, B5ZA72, Q97B25, B2G9H2, Q110Z9, Q5YP79, Q9KU97, Q5WIE9, B7HQM1, B0KJV9, A7GXK4, Q6D1Z0, A9I1R3, Q12WM7, B3R312, Q5E2W6, A9A875, A0QR33, A9KBA0, A0QLG2, B6J495, Q5QVP9, A8AAB3, C1KVK0, Q5WWG1, Q99T15, A1WBR8, C3P9E6, Q8RFY7, A5UML0, Q5NGB9, Q5UZ90, Q0HSE6, Q4UYA7, Q8ZBL9, B7KA18, A7X388, Q8Y6X8, Q8NT73, Q21MJ0, Q2LVW6, B2UX41, B9E7Y3, Q325Y5, A8FB92, A5UU40, Q2RJ31, C1AZ30, Q3K6C0, Q62HV8, C4K6Y5, Q6GG38, A0Q2A8, Q822Q0, A7NKV1, Q7M847, A0AJD9, Q65M82, Q9JXW0, A4SJ79, Q30RJ4, O29027, Q9CNG9, Q82UQ8, Q65U43, Q8Y1M4, A3PBK8, C3MYE0, A9MPK7, A4J6H0, P99096, Q2FFN1, A4JC86, A6LKX4, Q9HMY8, A0RJ78, A9AEU0, C3N842, Q8NVU6, A4FPX3, B4UKE6, B6JKN5, C0QQ98, A9B550, Q7U598, A0KZS6, A6T4V8, Q3KMF2, A0AJ02, B8JCU6, B0RBL3, Q81LD0, Q02SE5, A9L5J5, B2VE25</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>oxaloacetate</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>hopa</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>23.32996788924784</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.308047138047138</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.1463636363636364</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Q46N53</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Q9KJF0</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Q89QH2, A4YXN2, B3QBS6, Q8XBR7, B7M6P3, A4G242, A5EGD7, Q46S66, Q2IUI7, B1X9P6, Q31Y97, Q6N8F8, B1IX88, A7ZPI2, B1LMH0, Q217M3, Q46S72, A4G241, Q8FFE8, B6JE29, B7NPQ8, C4ZVR1, A7ICK2, B7UG84, Q0TF87, Q82M40, A6T0J2, B2TWX3, Q0K0H8, A9X6P7, O87838, Q3YZF6, B5YYX4, P69902, Q07Q82, Q1R8Z2, B6I6S5, A8A2M8, Q13RQ4, B7LBS7, P69903, O06644, B7MH34, Q32DG9, B7MY33, A1ADQ1, B7N5X4, Q139H7</t>
+          <t>G8FRC5</t>
         </is>
       </c>
     </row>

</xml_diff>